<commit_message>
Populated empty cells to 0 under #ELA Proficiency columns
</commit_message>
<xml_diff>
--- a/ela_proficiency_charter_schools_only.xlsx
+++ b/ela_proficiency_charter_schools_only.xlsx
@@ -569,9 +569,15 @@
       <c r="L2" t="n">
         <v>5</v>
       </c>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr"/>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0</v>
+      </c>
       <c r="P2" t="n">
         <v>0</v>
       </c>
@@ -628,9 +634,15 @@
       <c r="L3" t="n">
         <v>15</v>
       </c>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0</v>
+      </c>
       <c r="P3" t="n">
         <v>3</v>
       </c>
@@ -678,15 +690,27 @@
       <c r="I4" t="n">
         <v>8</v>
       </c>
-      <c r="J4" t="inlineStr"/>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
       <c r="K4" t="n">
         <v>7</v>
       </c>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
       <c r="Q4" t="n">
         <v>0</v>
       </c>
@@ -731,14 +755,24 @@
       <c r="I5" t="n">
         <v>22</v>
       </c>
-      <c r="J5" t="inlineStr"/>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
       <c r="K5" t="n">
         <v>36</v>
       </c>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0</v>
+      </c>
       <c r="P5" t="n">
         <v>4</v>
       </c>
@@ -783,16 +817,30 @@
       <c r="H6" t="n">
         <v>0</v>
       </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
       <c r="K6" t="n">
         <v>0</v>
       </c>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
-      <c r="P6" t="inlineStr"/>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0</v>
+      </c>
       <c r="Q6" t="n">
         <v>0</v>
       </c>
@@ -837,16 +885,30 @@
       <c r="I7" t="n">
         <v>1</v>
       </c>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
       <c r="L7" t="n">
         <v>5</v>
       </c>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
-      <c r="P7" t="inlineStr"/>
-      <c r="Q7" t="inlineStr"/>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -885,16 +947,30 @@
       <c r="H8" t="n">
         <v>3</v>
       </c>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
       <c r="K8" t="n">
         <v>3</v>
       </c>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
-      <c r="P8" t="inlineStr"/>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0</v>
+      </c>
       <c r="Q8" t="n">
         <v>0</v>
       </c>
@@ -939,17 +1015,27 @@
       <c r="I9" t="n">
         <v>0</v>
       </c>
-      <c r="J9" t="inlineStr"/>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
       <c r="K9" t="n">
         <v>0</v>
       </c>
       <c r="L9" t="n">
         <v>0</v>
       </c>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
-      <c r="P9" t="inlineStr"/>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0</v>
+      </c>
       <c r="Q9" t="n">
         <v>0</v>
       </c>
@@ -994,16 +1080,30 @@
       <c r="I10" t="n">
         <v>1</v>
       </c>
-      <c r="J10" t="inlineStr"/>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
       <c r="K10" t="n">
         <v>1</v>
       </c>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
-      <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="inlineStr"/>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1045,16 +1145,30 @@
       <c r="I11" t="n">
         <v>0</v>
       </c>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
       <c r="L11" t="n">
         <v>0</v>
       </c>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
-      <c r="P11" t="inlineStr"/>
-      <c r="Q11" t="inlineStr"/>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1105,10 +1219,18 @@
       <c r="L12" t="n">
         <v>56</v>
       </c>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
-      <c r="P12" t="inlineStr"/>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0</v>
+      </c>
       <c r="Q12" t="n">
         <v>10</v>
       </c>
@@ -1153,15 +1275,27 @@
       <c r="I13" t="n">
         <v>26</v>
       </c>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
       <c r="L13" t="n">
         <v>37</v>
       </c>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
-      <c r="P13" t="inlineStr"/>
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0</v>
+      </c>
       <c r="Q13" t="n">
         <v>3</v>
       </c>
@@ -1206,17 +1340,27 @@
       <c r="I14" t="n">
         <v>3</v>
       </c>
-      <c r="J14" t="inlineStr"/>
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
       <c r="K14" t="n">
         <v>1</v>
       </c>
       <c r="L14" t="n">
         <v>12</v>
       </c>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr"/>
-      <c r="P14" t="inlineStr"/>
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0</v>
+      </c>
       <c r="Q14" t="n">
         <v>3</v>
       </c>
@@ -1261,17 +1405,27 @@
       <c r="I15" t="n">
         <v>0</v>
       </c>
-      <c r="J15" t="inlineStr"/>
+      <c r="J15" t="n">
+        <v>0</v>
+      </c>
       <c r="K15" t="n">
         <v>0</v>
       </c>
       <c r="L15" t="n">
         <v>0</v>
       </c>
-      <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr"/>
-      <c r="O15" t="inlineStr"/>
-      <c r="P15" t="inlineStr"/>
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0</v>
+      </c>
       <c r="Q15" t="n">
         <v>0</v>
       </c>
@@ -1316,17 +1470,27 @@
       <c r="I16" t="n">
         <v>7</v>
       </c>
-      <c r="J16" t="inlineStr"/>
+      <c r="J16" t="n">
+        <v>0</v>
+      </c>
       <c r="K16" t="n">
         <v>4</v>
       </c>
       <c r="L16" t="n">
         <v>14</v>
       </c>
-      <c r="M16" t="inlineStr"/>
-      <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr"/>
-      <c r="P16" t="inlineStr"/>
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0</v>
+      </c>
       <c r="Q16" t="n">
         <v>1</v>
       </c>
@@ -1371,16 +1535,24 @@
       <c r="I17" t="n">
         <v>53</v>
       </c>
-      <c r="J17" t="inlineStr"/>
+      <c r="J17" t="n">
+        <v>0</v>
+      </c>
       <c r="K17" t="n">
         <v>70</v>
       </c>
       <c r="L17" t="n">
         <v>4</v>
       </c>
-      <c r="M17" t="inlineStr"/>
-      <c r="N17" t="inlineStr"/>
-      <c r="O17" t="inlineStr"/>
+      <c r="M17" t="n">
+        <v>0</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0</v>
+      </c>
       <c r="P17" t="n">
         <v>2</v>
       </c>
@@ -1428,17 +1600,27 @@
       <c r="I18" t="n">
         <v>19</v>
       </c>
-      <c r="J18" t="inlineStr"/>
+      <c r="J18" t="n">
+        <v>0</v>
+      </c>
       <c r="K18" t="n">
         <v>5</v>
       </c>
       <c r="L18" t="n">
         <v>22</v>
       </c>
-      <c r="M18" t="inlineStr"/>
-      <c r="N18" t="inlineStr"/>
-      <c r="O18" t="inlineStr"/>
-      <c r="P18" t="inlineStr"/>
+      <c r="M18" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0</v>
+      </c>
       <c r="Q18" t="n">
         <v>6</v>
       </c>
@@ -1483,17 +1665,27 @@
       <c r="I19" t="n">
         <v>11</v>
       </c>
-      <c r="J19" t="inlineStr"/>
+      <c r="J19" t="n">
+        <v>0</v>
+      </c>
       <c r="K19" t="n">
         <v>5</v>
       </c>
       <c r="L19" t="n">
         <v>19</v>
       </c>
-      <c r="M19" t="inlineStr"/>
-      <c r="N19" t="inlineStr"/>
-      <c r="O19" t="inlineStr"/>
-      <c r="P19" t="inlineStr"/>
+      <c r="M19" t="n">
+        <v>0</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0</v>
+      </c>
+      <c r="O19" t="n">
+        <v>0</v>
+      </c>
+      <c r="P19" t="n">
+        <v>0</v>
+      </c>
       <c r="Q19" t="n">
         <v>2</v>
       </c>
@@ -1538,7 +1730,9 @@
       <c r="I20" t="n">
         <v>20</v>
       </c>
-      <c r="J20" t="inlineStr"/>
+      <c r="J20" t="n">
+        <v>0</v>
+      </c>
       <c r="K20" t="n">
         <v>4</v>
       </c>
@@ -1548,9 +1742,15 @@
       <c r="M20" t="n">
         <v>5</v>
       </c>
-      <c r="N20" t="inlineStr"/>
-      <c r="O20" t="inlineStr"/>
-      <c r="P20" t="inlineStr"/>
+      <c r="N20" t="n">
+        <v>0</v>
+      </c>
+      <c r="O20" t="n">
+        <v>0</v>
+      </c>
+      <c r="P20" t="n">
+        <v>0</v>
+      </c>
       <c r="Q20" t="n">
         <v>2</v>
       </c>
@@ -1595,15 +1795,27 @@
       <c r="I21" t="n">
         <v>1</v>
       </c>
-      <c r="J21" t="inlineStr"/>
+      <c r="J21" t="n">
+        <v>0</v>
+      </c>
       <c r="K21" t="n">
         <v>5</v>
       </c>
-      <c r="L21" t="inlineStr"/>
-      <c r="M21" t="inlineStr"/>
-      <c r="N21" t="inlineStr"/>
-      <c r="O21" t="inlineStr"/>
-      <c r="P21" t="inlineStr"/>
+      <c r="L21" t="n">
+        <v>0</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0</v>
+      </c>
+      <c r="N21" t="n">
+        <v>0</v>
+      </c>
+      <c r="O21" t="n">
+        <v>0</v>
+      </c>
+      <c r="P21" t="n">
+        <v>0</v>
+      </c>
       <c r="Q21" t="n">
         <v>1</v>
       </c>
@@ -1648,15 +1860,27 @@
       <c r="I22" t="n">
         <v>2</v>
       </c>
-      <c r="J22" t="inlineStr"/>
+      <c r="J22" t="n">
+        <v>0</v>
+      </c>
       <c r="K22" t="n">
         <v>3</v>
       </c>
-      <c r="L22" t="inlineStr"/>
-      <c r="M22" t="inlineStr"/>
-      <c r="N22" t="inlineStr"/>
-      <c r="O22" t="inlineStr"/>
-      <c r="P22" t="inlineStr"/>
+      <c r="L22" t="n">
+        <v>0</v>
+      </c>
+      <c r="M22" t="n">
+        <v>0</v>
+      </c>
+      <c r="N22" t="n">
+        <v>0</v>
+      </c>
+      <c r="O22" t="n">
+        <v>0</v>
+      </c>
+      <c r="P22" t="n">
+        <v>0</v>
+      </c>
       <c r="Q22" t="n">
         <v>1</v>
       </c>
@@ -1701,15 +1925,27 @@
       <c r="I23" t="n">
         <v>3</v>
       </c>
-      <c r="J23" t="inlineStr"/>
+      <c r="J23" t="n">
+        <v>0</v>
+      </c>
       <c r="K23" t="n">
         <v>3</v>
       </c>
-      <c r="L23" t="inlineStr"/>
-      <c r="M23" t="inlineStr"/>
-      <c r="N23" t="inlineStr"/>
-      <c r="O23" t="inlineStr"/>
-      <c r="P23" t="inlineStr"/>
+      <c r="L23" t="n">
+        <v>0</v>
+      </c>
+      <c r="M23" t="n">
+        <v>0</v>
+      </c>
+      <c r="N23" t="n">
+        <v>0</v>
+      </c>
+      <c r="O23" t="n">
+        <v>0</v>
+      </c>
+      <c r="P23" t="n">
+        <v>0</v>
+      </c>
       <c r="Q23" t="n">
         <v>0</v>
       </c>
@@ -1754,15 +1990,27 @@
       <c r="I24" t="n">
         <v>4</v>
       </c>
-      <c r="J24" t="inlineStr"/>
+      <c r="J24" t="n">
+        <v>0</v>
+      </c>
       <c r="K24" t="n">
         <v>7</v>
       </c>
-      <c r="L24" t="inlineStr"/>
-      <c r="M24" t="inlineStr"/>
-      <c r="N24" t="inlineStr"/>
-      <c r="O24" t="inlineStr"/>
-      <c r="P24" t="inlineStr"/>
+      <c r="L24" t="n">
+        <v>0</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0</v>
+      </c>
+      <c r="N24" t="n">
+        <v>0</v>
+      </c>
+      <c r="O24" t="n">
+        <v>0</v>
+      </c>
+      <c r="P24" t="n">
+        <v>0</v>
+      </c>
       <c r="Q24" t="n">
         <v>0</v>
       </c>
@@ -1807,15 +2055,27 @@
       <c r="I25" t="n">
         <v>3</v>
       </c>
-      <c r="J25" t="inlineStr"/>
+      <c r="J25" t="n">
+        <v>0</v>
+      </c>
       <c r="K25" t="n">
         <v>3</v>
       </c>
-      <c r="L25" t="inlineStr"/>
-      <c r="M25" t="inlineStr"/>
-      <c r="N25" t="inlineStr"/>
-      <c r="O25" t="inlineStr"/>
-      <c r="P25" t="inlineStr"/>
+      <c r="L25" t="n">
+        <v>0</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0</v>
+      </c>
+      <c r="N25" t="n">
+        <v>0</v>
+      </c>
+      <c r="O25" t="n">
+        <v>0</v>
+      </c>
+      <c r="P25" t="n">
+        <v>0</v>
+      </c>
       <c r="Q25" t="n">
         <v>1</v>
       </c>
@@ -1860,17 +2120,27 @@
       <c r="I26" t="n">
         <v>9</v>
       </c>
-      <c r="J26" t="inlineStr"/>
+      <c r="J26" t="n">
+        <v>0</v>
+      </c>
       <c r="K26" t="n">
         <v>5</v>
       </c>
       <c r="L26" t="n">
         <v>19</v>
       </c>
-      <c r="M26" t="inlineStr"/>
-      <c r="N26" t="inlineStr"/>
-      <c r="O26" t="inlineStr"/>
-      <c r="P26" t="inlineStr"/>
+      <c r="M26" t="n">
+        <v>0</v>
+      </c>
+      <c r="N26" t="n">
+        <v>0</v>
+      </c>
+      <c r="O26" t="n">
+        <v>0</v>
+      </c>
+      <c r="P26" t="n">
+        <v>0</v>
+      </c>
       <c r="Q26" t="n">
         <v>5</v>
       </c>
@@ -1915,17 +2185,27 @@
       <c r="I27" t="n">
         <v>18</v>
       </c>
-      <c r="J27" t="inlineStr"/>
+      <c r="J27" t="n">
+        <v>0</v>
+      </c>
       <c r="K27" t="n">
         <v>1</v>
       </c>
       <c r="L27" t="n">
         <v>32</v>
       </c>
-      <c r="M27" t="inlineStr"/>
-      <c r="N27" t="inlineStr"/>
-      <c r="O27" t="inlineStr"/>
-      <c r="P27" t="inlineStr"/>
+      <c r="M27" t="n">
+        <v>0</v>
+      </c>
+      <c r="N27" t="n">
+        <v>0</v>
+      </c>
+      <c r="O27" t="n">
+        <v>0</v>
+      </c>
+      <c r="P27" t="n">
+        <v>0</v>
+      </c>
       <c r="Q27" t="n">
         <v>3</v>
       </c>
@@ -1970,17 +2250,27 @@
       <c r="I28" t="n">
         <v>7</v>
       </c>
-      <c r="J28" t="inlineStr"/>
+      <c r="J28" t="n">
+        <v>0</v>
+      </c>
       <c r="K28" t="n">
         <v>4</v>
       </c>
       <c r="L28" t="n">
         <v>12</v>
       </c>
-      <c r="M28" t="inlineStr"/>
-      <c r="N28" t="inlineStr"/>
-      <c r="O28" t="inlineStr"/>
-      <c r="P28" t="inlineStr"/>
+      <c r="M28" t="n">
+        <v>0</v>
+      </c>
+      <c r="N28" t="n">
+        <v>0</v>
+      </c>
+      <c r="O28" t="n">
+        <v>0</v>
+      </c>
+      <c r="P28" t="n">
+        <v>0</v>
+      </c>
       <c r="Q28" t="n">
         <v>0</v>
       </c>
@@ -2025,15 +2315,27 @@
       <c r="I29" t="n">
         <v>22</v>
       </c>
-      <c r="J29" t="inlineStr"/>
-      <c r="K29" t="inlineStr"/>
+      <c r="J29" t="n">
+        <v>0</v>
+      </c>
+      <c r="K29" t="n">
+        <v>0</v>
+      </c>
       <c r="L29" t="n">
         <v>35</v>
       </c>
-      <c r="M29" t="inlineStr"/>
-      <c r="N29" t="inlineStr"/>
-      <c r="O29" t="inlineStr"/>
-      <c r="P29" t="inlineStr"/>
+      <c r="M29" t="n">
+        <v>0</v>
+      </c>
+      <c r="N29" t="n">
+        <v>0</v>
+      </c>
+      <c r="O29" t="n">
+        <v>0</v>
+      </c>
+      <c r="P29" t="n">
+        <v>0</v>
+      </c>
       <c r="Q29" t="n">
         <v>3</v>
       </c>
@@ -2078,15 +2380,27 @@
       <c r="I30" t="n">
         <v>0</v>
       </c>
-      <c r="J30" t="inlineStr"/>
+      <c r="J30" t="n">
+        <v>0</v>
+      </c>
       <c r="K30" t="n">
         <v>0</v>
       </c>
-      <c r="L30" t="inlineStr"/>
-      <c r="M30" t="inlineStr"/>
-      <c r="N30" t="inlineStr"/>
-      <c r="O30" t="inlineStr"/>
-      <c r="P30" t="inlineStr"/>
+      <c r="L30" t="n">
+        <v>0</v>
+      </c>
+      <c r="M30" t="n">
+        <v>0</v>
+      </c>
+      <c r="N30" t="n">
+        <v>0</v>
+      </c>
+      <c r="O30" t="n">
+        <v>0</v>
+      </c>
+      <c r="P30" t="n">
+        <v>0</v>
+      </c>
       <c r="Q30" t="n">
         <v>0</v>
       </c>
@@ -2131,17 +2445,27 @@
       <c r="I31" t="n">
         <v>18</v>
       </c>
-      <c r="J31" t="inlineStr"/>
+      <c r="J31" t="n">
+        <v>0</v>
+      </c>
       <c r="K31" t="n">
         <v>27</v>
       </c>
       <c r="L31" t="n">
         <v>7</v>
       </c>
-      <c r="M31" t="inlineStr"/>
-      <c r="N31" t="inlineStr"/>
-      <c r="O31" t="inlineStr"/>
-      <c r="P31" t="inlineStr"/>
+      <c r="M31" t="n">
+        <v>0</v>
+      </c>
+      <c r="N31" t="n">
+        <v>0</v>
+      </c>
+      <c r="O31" t="n">
+        <v>0</v>
+      </c>
+      <c r="P31" t="n">
+        <v>0</v>
+      </c>
       <c r="Q31" t="n">
         <v>7</v>
       </c>
@@ -2186,15 +2510,27 @@
       <c r="I32" t="n">
         <v>4</v>
       </c>
-      <c r="J32" t="inlineStr"/>
+      <c r="J32" t="n">
+        <v>0</v>
+      </c>
       <c r="K32" t="n">
         <v>7</v>
       </c>
-      <c r="L32" t="inlineStr"/>
-      <c r="M32" t="inlineStr"/>
-      <c r="N32" t="inlineStr"/>
-      <c r="O32" t="inlineStr"/>
-      <c r="P32" t="inlineStr"/>
+      <c r="L32" t="n">
+        <v>0</v>
+      </c>
+      <c r="M32" t="n">
+        <v>0</v>
+      </c>
+      <c r="N32" t="n">
+        <v>0</v>
+      </c>
+      <c r="O32" t="n">
+        <v>0</v>
+      </c>
+      <c r="P32" t="n">
+        <v>0</v>
+      </c>
       <c r="Q32" t="n">
         <v>0</v>
       </c>
@@ -2239,15 +2575,27 @@
       <c r="I33" t="n">
         <v>24</v>
       </c>
-      <c r="J33" t="inlineStr"/>
+      <c r="J33" t="n">
+        <v>0</v>
+      </c>
       <c r="K33" t="n">
         <v>28</v>
       </c>
-      <c r="L33" t="inlineStr"/>
-      <c r="M33" t="inlineStr"/>
-      <c r="N33" t="inlineStr"/>
-      <c r="O33" t="inlineStr"/>
-      <c r="P33" t="inlineStr"/>
+      <c r="L33" t="n">
+        <v>0</v>
+      </c>
+      <c r="M33" t="n">
+        <v>0</v>
+      </c>
+      <c r="N33" t="n">
+        <v>0</v>
+      </c>
+      <c r="O33" t="n">
+        <v>0</v>
+      </c>
+      <c r="P33" t="n">
+        <v>0</v>
+      </c>
       <c r="Q33" t="n">
         <v>1</v>
       </c>
@@ -2292,15 +2640,27 @@
       <c r="I34" t="n">
         <v>2</v>
       </c>
-      <c r="J34" t="inlineStr"/>
+      <c r="J34" t="n">
+        <v>0</v>
+      </c>
       <c r="K34" t="n">
         <v>2</v>
       </c>
-      <c r="L34" t="inlineStr"/>
-      <c r="M34" t="inlineStr"/>
-      <c r="N34" t="inlineStr"/>
-      <c r="O34" t="inlineStr"/>
-      <c r="P34" t="inlineStr"/>
+      <c r="L34" t="n">
+        <v>0</v>
+      </c>
+      <c r="M34" t="n">
+        <v>0</v>
+      </c>
+      <c r="N34" t="n">
+        <v>0</v>
+      </c>
+      <c r="O34" t="n">
+        <v>0</v>
+      </c>
+      <c r="P34" t="n">
+        <v>0</v>
+      </c>
       <c r="Q34" t="n">
         <v>1</v>
       </c>
@@ -2345,15 +2705,27 @@
       <c r="I35" t="n">
         <v>3</v>
       </c>
-      <c r="J35" t="inlineStr"/>
+      <c r="J35" t="n">
+        <v>0</v>
+      </c>
       <c r="K35" t="n">
         <v>4</v>
       </c>
-      <c r="L35" t="inlineStr"/>
-      <c r="M35" t="inlineStr"/>
-      <c r="N35" t="inlineStr"/>
-      <c r="O35" t="inlineStr"/>
-      <c r="P35" t="inlineStr"/>
+      <c r="L35" t="n">
+        <v>0</v>
+      </c>
+      <c r="M35" t="n">
+        <v>0</v>
+      </c>
+      <c r="N35" t="n">
+        <v>0</v>
+      </c>
+      <c r="O35" t="n">
+        <v>0</v>
+      </c>
+      <c r="P35" t="n">
+        <v>0</v>
+      </c>
       <c r="Q35" t="n">
         <v>0</v>
       </c>
@@ -2398,16 +2770,30 @@
       <c r="I36" t="n">
         <v>0</v>
       </c>
-      <c r="J36" t="inlineStr"/>
+      <c r="J36" t="n">
+        <v>0</v>
+      </c>
       <c r="K36" t="n">
         <v>0</v>
       </c>
-      <c r="L36" t="inlineStr"/>
-      <c r="M36" t="inlineStr"/>
-      <c r="N36" t="inlineStr"/>
-      <c r="O36" t="inlineStr"/>
-      <c r="P36" t="inlineStr"/>
-      <c r="Q36" t="inlineStr"/>
+      <c r="L36" t="n">
+        <v>0</v>
+      </c>
+      <c r="M36" t="n">
+        <v>0</v>
+      </c>
+      <c r="N36" t="n">
+        <v>0</v>
+      </c>
+      <c r="O36" t="n">
+        <v>0</v>
+      </c>
+      <c r="P36" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -2449,16 +2835,30 @@
       <c r="I37" t="n">
         <v>0</v>
       </c>
-      <c r="J37" t="inlineStr"/>
+      <c r="J37" t="n">
+        <v>0</v>
+      </c>
       <c r="K37" t="n">
         <v>0</v>
       </c>
-      <c r="L37" t="inlineStr"/>
-      <c r="M37" t="inlineStr"/>
-      <c r="N37" t="inlineStr"/>
-      <c r="O37" t="inlineStr"/>
-      <c r="P37" t="inlineStr"/>
-      <c r="Q37" t="inlineStr"/>
+      <c r="L37" t="n">
+        <v>0</v>
+      </c>
+      <c r="M37" t="n">
+        <v>0</v>
+      </c>
+      <c r="N37" t="n">
+        <v>0</v>
+      </c>
+      <c r="O37" t="n">
+        <v>0</v>
+      </c>
+      <c r="P37" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2500,17 +2900,27 @@
       <c r="I38" t="n">
         <v>0</v>
       </c>
-      <c r="J38" t="inlineStr"/>
+      <c r="J38" t="n">
+        <v>0</v>
+      </c>
       <c r="K38" t="n">
         <v>0</v>
       </c>
       <c r="L38" t="n">
         <v>2</v>
       </c>
-      <c r="M38" t="inlineStr"/>
-      <c r="N38" t="inlineStr"/>
-      <c r="O38" t="inlineStr"/>
-      <c r="P38" t="inlineStr"/>
+      <c r="M38" t="n">
+        <v>0</v>
+      </c>
+      <c r="N38" t="n">
+        <v>0</v>
+      </c>
+      <c r="O38" t="n">
+        <v>0</v>
+      </c>
+      <c r="P38" t="n">
+        <v>0</v>
+      </c>
       <c r="Q38" t="n">
         <v>0</v>
       </c>
@@ -2549,20 +2959,36 @@
       <c r="G39" t="n">
         <v>0</v>
       </c>
-      <c r="H39" t="inlineStr"/>
+      <c r="H39" t="n">
+        <v>0</v>
+      </c>
       <c r="I39" t="n">
         <v>0</v>
       </c>
-      <c r="J39" t="inlineStr"/>
-      <c r="K39" t="inlineStr"/>
+      <c r="J39" t="n">
+        <v>0</v>
+      </c>
+      <c r="K39" t="n">
+        <v>0</v>
+      </c>
       <c r="L39" t="n">
         <v>0</v>
       </c>
-      <c r="M39" t="inlineStr"/>
-      <c r="N39" t="inlineStr"/>
-      <c r="O39" t="inlineStr"/>
-      <c r="P39" t="inlineStr"/>
-      <c r="Q39" t="inlineStr"/>
+      <c r="M39" t="n">
+        <v>0</v>
+      </c>
+      <c r="N39" t="n">
+        <v>0</v>
+      </c>
+      <c r="O39" t="n">
+        <v>0</v>
+      </c>
+      <c r="P39" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q39" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2604,15 +3030,27 @@
       <c r="I40" t="n">
         <v>0</v>
       </c>
-      <c r="J40" t="inlineStr"/>
+      <c r="J40" t="n">
+        <v>0</v>
+      </c>
       <c r="K40" t="n">
         <v>0</v>
       </c>
-      <c r="L40" t="inlineStr"/>
-      <c r="M40" t="inlineStr"/>
-      <c r="N40" t="inlineStr"/>
-      <c r="O40" t="inlineStr"/>
-      <c r="P40" t="inlineStr"/>
+      <c r="L40" t="n">
+        <v>0</v>
+      </c>
+      <c r="M40" t="n">
+        <v>0</v>
+      </c>
+      <c r="N40" t="n">
+        <v>0</v>
+      </c>
+      <c r="O40" t="n">
+        <v>0</v>
+      </c>
+      <c r="P40" t="n">
+        <v>0</v>
+      </c>
       <c r="Q40" t="n">
         <v>0</v>
       </c>
@@ -2657,15 +3095,27 @@
       <c r="I41" t="n">
         <v>0</v>
       </c>
-      <c r="J41" t="inlineStr"/>
+      <c r="J41" t="n">
+        <v>0</v>
+      </c>
       <c r="K41" t="n">
         <v>0</v>
       </c>
-      <c r="L41" t="inlineStr"/>
-      <c r="M41" t="inlineStr"/>
-      <c r="N41" t="inlineStr"/>
-      <c r="O41" t="inlineStr"/>
-      <c r="P41" t="inlineStr"/>
+      <c r="L41" t="n">
+        <v>0</v>
+      </c>
+      <c r="M41" t="n">
+        <v>0</v>
+      </c>
+      <c r="N41" t="n">
+        <v>0</v>
+      </c>
+      <c r="O41" t="n">
+        <v>0</v>
+      </c>
+      <c r="P41" t="n">
+        <v>0</v>
+      </c>
       <c r="Q41" t="n">
         <v>0</v>
       </c>
@@ -2710,16 +3160,30 @@
       <c r="I42" t="n">
         <v>0</v>
       </c>
-      <c r="J42" t="inlineStr"/>
+      <c r="J42" t="n">
+        <v>0</v>
+      </c>
       <c r="K42" t="n">
         <v>0</v>
       </c>
-      <c r="L42" t="inlineStr"/>
-      <c r="M42" t="inlineStr"/>
-      <c r="N42" t="inlineStr"/>
-      <c r="O42" t="inlineStr"/>
-      <c r="P42" t="inlineStr"/>
-      <c r="Q42" t="inlineStr"/>
+      <c r="L42" t="n">
+        <v>0</v>
+      </c>
+      <c r="M42" t="n">
+        <v>0</v>
+      </c>
+      <c r="N42" t="n">
+        <v>0</v>
+      </c>
+      <c r="O42" t="n">
+        <v>0</v>
+      </c>
+      <c r="P42" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q42" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2761,17 +3225,27 @@
       <c r="I43" t="n">
         <v>0</v>
       </c>
-      <c r="J43" t="inlineStr"/>
+      <c r="J43" t="n">
+        <v>0</v>
+      </c>
       <c r="K43" t="n">
         <v>0</v>
       </c>
       <c r="L43" t="n">
         <v>0</v>
       </c>
-      <c r="M43" t="inlineStr"/>
-      <c r="N43" t="inlineStr"/>
-      <c r="O43" t="inlineStr"/>
-      <c r="P43" t="inlineStr"/>
+      <c r="M43" t="n">
+        <v>0</v>
+      </c>
+      <c r="N43" t="n">
+        <v>0</v>
+      </c>
+      <c r="O43" t="n">
+        <v>0</v>
+      </c>
+      <c r="P43" t="n">
+        <v>0</v>
+      </c>
       <c r="Q43" t="n">
         <v>0</v>
       </c>
@@ -2816,17 +3290,27 @@
       <c r="I44" t="n">
         <v>0</v>
       </c>
-      <c r="J44" t="inlineStr"/>
+      <c r="J44" t="n">
+        <v>0</v>
+      </c>
       <c r="K44" t="n">
         <v>0</v>
       </c>
       <c r="L44" t="n">
         <v>0</v>
       </c>
-      <c r="M44" t="inlineStr"/>
-      <c r="N44" t="inlineStr"/>
-      <c r="O44" t="inlineStr"/>
-      <c r="P44" t="inlineStr"/>
+      <c r="M44" t="n">
+        <v>0</v>
+      </c>
+      <c r="N44" t="n">
+        <v>0</v>
+      </c>
+      <c r="O44" t="n">
+        <v>0</v>
+      </c>
+      <c r="P44" t="n">
+        <v>0</v>
+      </c>
       <c r="Q44" t="n">
         <v>0</v>
       </c>
@@ -2871,16 +3355,30 @@
       <c r="I45" t="n">
         <v>0</v>
       </c>
-      <c r="J45" t="inlineStr"/>
-      <c r="K45" t="inlineStr"/>
+      <c r="J45" t="n">
+        <v>0</v>
+      </c>
+      <c r="K45" t="n">
+        <v>0</v>
+      </c>
       <c r="L45" t="n">
         <v>0</v>
       </c>
-      <c r="M45" t="inlineStr"/>
-      <c r="N45" t="inlineStr"/>
-      <c r="O45" t="inlineStr"/>
-      <c r="P45" t="inlineStr"/>
-      <c r="Q45" t="inlineStr"/>
+      <c r="M45" t="n">
+        <v>0</v>
+      </c>
+      <c r="N45" t="n">
+        <v>0</v>
+      </c>
+      <c r="O45" t="n">
+        <v>0</v>
+      </c>
+      <c r="P45" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q45" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2922,16 +3420,30 @@
       <c r="I46" t="n">
         <v>0</v>
       </c>
-      <c r="J46" t="inlineStr"/>
+      <c r="J46" t="n">
+        <v>0</v>
+      </c>
       <c r="K46" t="n">
         <v>0</v>
       </c>
-      <c r="L46" t="inlineStr"/>
-      <c r="M46" t="inlineStr"/>
-      <c r="N46" t="inlineStr"/>
-      <c r="O46" t="inlineStr"/>
-      <c r="P46" t="inlineStr"/>
-      <c r="Q46" t="inlineStr"/>
+      <c r="L46" t="n">
+        <v>0</v>
+      </c>
+      <c r="M46" t="n">
+        <v>0</v>
+      </c>
+      <c r="N46" t="n">
+        <v>0</v>
+      </c>
+      <c r="O46" t="n">
+        <v>0</v>
+      </c>
+      <c r="P46" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q46" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2973,15 +3485,27 @@
       <c r="I47" t="n">
         <v>1</v>
       </c>
-      <c r="J47" t="inlineStr"/>
+      <c r="J47" t="n">
+        <v>0</v>
+      </c>
       <c r="K47" t="n">
         <v>1</v>
       </c>
-      <c r="L47" t="inlineStr"/>
-      <c r="M47" t="inlineStr"/>
-      <c r="N47" t="inlineStr"/>
-      <c r="O47" t="inlineStr"/>
-      <c r="P47" t="inlineStr"/>
+      <c r="L47" t="n">
+        <v>0</v>
+      </c>
+      <c r="M47" t="n">
+        <v>0</v>
+      </c>
+      <c r="N47" t="n">
+        <v>0</v>
+      </c>
+      <c r="O47" t="n">
+        <v>0</v>
+      </c>
+      <c r="P47" t="n">
+        <v>0</v>
+      </c>
       <c r="Q47" t="n">
         <v>0</v>
       </c>
@@ -3026,18 +3550,30 @@
       <c r="I48" t="n">
         <v>2</v>
       </c>
-      <c r="J48" t="inlineStr"/>
+      <c r="J48" t="n">
+        <v>0</v>
+      </c>
       <c r="K48" t="n">
         <v>1</v>
       </c>
       <c r="L48" t="n">
         <v>0</v>
       </c>
-      <c r="M48" t="inlineStr"/>
-      <c r="N48" t="inlineStr"/>
-      <c r="O48" t="inlineStr"/>
-      <c r="P48" t="inlineStr"/>
-      <c r="Q48" t="inlineStr"/>
+      <c r="M48" t="n">
+        <v>0</v>
+      </c>
+      <c r="N48" t="n">
+        <v>0</v>
+      </c>
+      <c r="O48" t="n">
+        <v>0</v>
+      </c>
+      <c r="P48" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q48" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -3079,15 +3615,27 @@
       <c r="I49" t="n">
         <v>1</v>
       </c>
-      <c r="J49" t="inlineStr"/>
+      <c r="J49" t="n">
+        <v>0</v>
+      </c>
       <c r="K49" t="n">
         <v>1</v>
       </c>
-      <c r="L49" t="inlineStr"/>
-      <c r="M49" t="inlineStr"/>
-      <c r="N49" t="inlineStr"/>
-      <c r="O49" t="inlineStr"/>
-      <c r="P49" t="inlineStr"/>
+      <c r="L49" t="n">
+        <v>0</v>
+      </c>
+      <c r="M49" t="n">
+        <v>0</v>
+      </c>
+      <c r="N49" t="n">
+        <v>0</v>
+      </c>
+      <c r="O49" t="n">
+        <v>0</v>
+      </c>
+      <c r="P49" t="n">
+        <v>0</v>
+      </c>
       <c r="Q49" t="n">
         <v>0</v>
       </c>
@@ -3132,15 +3680,27 @@
       <c r="I50" t="n">
         <v>0</v>
       </c>
-      <c r="J50" t="inlineStr"/>
+      <c r="J50" t="n">
+        <v>0</v>
+      </c>
       <c r="K50" t="n">
         <v>0</v>
       </c>
-      <c r="L50" t="inlineStr"/>
-      <c r="M50" t="inlineStr"/>
-      <c r="N50" t="inlineStr"/>
-      <c r="O50" t="inlineStr"/>
-      <c r="P50" t="inlineStr"/>
+      <c r="L50" t="n">
+        <v>0</v>
+      </c>
+      <c r="M50" t="n">
+        <v>0</v>
+      </c>
+      <c r="N50" t="n">
+        <v>0</v>
+      </c>
+      <c r="O50" t="n">
+        <v>0</v>
+      </c>
+      <c r="P50" t="n">
+        <v>0</v>
+      </c>
       <c r="Q50" t="n">
         <v>0</v>
       </c>
@@ -3185,15 +3745,27 @@
       <c r="I51" t="n">
         <v>0</v>
       </c>
-      <c r="J51" t="inlineStr"/>
+      <c r="J51" t="n">
+        <v>0</v>
+      </c>
       <c r="K51" t="n">
         <v>1</v>
       </c>
-      <c r="L51" t="inlineStr"/>
-      <c r="M51" t="inlineStr"/>
-      <c r="N51" t="inlineStr"/>
-      <c r="O51" t="inlineStr"/>
-      <c r="P51" t="inlineStr"/>
+      <c r="L51" t="n">
+        <v>0</v>
+      </c>
+      <c r="M51" t="n">
+        <v>0</v>
+      </c>
+      <c r="N51" t="n">
+        <v>0</v>
+      </c>
+      <c r="O51" t="n">
+        <v>0</v>
+      </c>
+      <c r="P51" t="n">
+        <v>0</v>
+      </c>
       <c r="Q51" t="n">
         <v>0</v>
       </c>
@@ -3238,15 +3810,27 @@
       <c r="I52" t="n">
         <v>0</v>
       </c>
-      <c r="J52" t="inlineStr"/>
+      <c r="J52" t="n">
+        <v>0</v>
+      </c>
       <c r="K52" t="n">
         <v>0</v>
       </c>
-      <c r="L52" t="inlineStr"/>
-      <c r="M52" t="inlineStr"/>
-      <c r="N52" t="inlineStr"/>
-      <c r="O52" t="inlineStr"/>
-      <c r="P52" t="inlineStr"/>
+      <c r="L52" t="n">
+        <v>0</v>
+      </c>
+      <c r="M52" t="n">
+        <v>0</v>
+      </c>
+      <c r="N52" t="n">
+        <v>0</v>
+      </c>
+      <c r="O52" t="n">
+        <v>0</v>
+      </c>
+      <c r="P52" t="n">
+        <v>0</v>
+      </c>
       <c r="Q52" t="n">
         <v>0</v>
       </c>
@@ -3291,15 +3875,27 @@
       <c r="I53" t="n">
         <v>0</v>
       </c>
-      <c r="J53" t="inlineStr"/>
-      <c r="K53" t="inlineStr"/>
+      <c r="J53" t="n">
+        <v>0</v>
+      </c>
+      <c r="K53" t="n">
+        <v>0</v>
+      </c>
       <c r="L53" t="n">
         <v>2</v>
       </c>
-      <c r="M53" t="inlineStr"/>
-      <c r="N53" t="inlineStr"/>
-      <c r="O53" t="inlineStr"/>
-      <c r="P53" t="inlineStr"/>
+      <c r="M53" t="n">
+        <v>0</v>
+      </c>
+      <c r="N53" t="n">
+        <v>0</v>
+      </c>
+      <c r="O53" t="n">
+        <v>0</v>
+      </c>
+      <c r="P53" t="n">
+        <v>0</v>
+      </c>
       <c r="Q53" t="n">
         <v>1</v>
       </c>
@@ -3344,15 +3940,27 @@
       <c r="I54" t="n">
         <v>3</v>
       </c>
-      <c r="J54" t="inlineStr"/>
-      <c r="K54" t="inlineStr"/>
+      <c r="J54" t="n">
+        <v>0</v>
+      </c>
+      <c r="K54" t="n">
+        <v>0</v>
+      </c>
       <c r="L54" t="n">
         <v>4</v>
       </c>
-      <c r="M54" t="inlineStr"/>
-      <c r="N54" t="inlineStr"/>
-      <c r="O54" t="inlineStr"/>
-      <c r="P54" t="inlineStr"/>
+      <c r="M54" t="n">
+        <v>0</v>
+      </c>
+      <c r="N54" t="n">
+        <v>0</v>
+      </c>
+      <c r="O54" t="n">
+        <v>0</v>
+      </c>
+      <c r="P54" t="n">
+        <v>0</v>
+      </c>
       <c r="Q54" t="n">
         <v>0</v>
       </c>
@@ -3409,9 +4017,15 @@
       <c r="M55" t="n">
         <v>5</v>
       </c>
-      <c r="N55" t="inlineStr"/>
-      <c r="O55" t="inlineStr"/>
-      <c r="P55" t="inlineStr"/>
+      <c r="N55" t="n">
+        <v>0</v>
+      </c>
+      <c r="O55" t="n">
+        <v>0</v>
+      </c>
+      <c r="P55" t="n">
+        <v>0</v>
+      </c>
       <c r="Q55" t="n">
         <v>7</v>
       </c>
@@ -3456,15 +4070,27 @@
       <c r="I56" t="n">
         <v>0</v>
       </c>
-      <c r="J56" t="inlineStr"/>
+      <c r="J56" t="n">
+        <v>0</v>
+      </c>
       <c r="K56" t="n">
         <v>0</v>
       </c>
-      <c r="L56" t="inlineStr"/>
-      <c r="M56" t="inlineStr"/>
-      <c r="N56" t="inlineStr"/>
-      <c r="O56" t="inlineStr"/>
-      <c r="P56" t="inlineStr"/>
+      <c r="L56" t="n">
+        <v>0</v>
+      </c>
+      <c r="M56" t="n">
+        <v>0</v>
+      </c>
+      <c r="N56" t="n">
+        <v>0</v>
+      </c>
+      <c r="O56" t="n">
+        <v>0</v>
+      </c>
+      <c r="P56" t="n">
+        <v>0</v>
+      </c>
       <c r="Q56" t="n">
         <v>0</v>
       </c>
@@ -3509,15 +4135,27 @@
       <c r="I57" t="n">
         <v>1</v>
       </c>
-      <c r="J57" t="inlineStr"/>
+      <c r="J57" t="n">
+        <v>0</v>
+      </c>
       <c r="K57" t="n">
         <v>1</v>
       </c>
-      <c r="L57" t="inlineStr"/>
-      <c r="M57" t="inlineStr"/>
-      <c r="N57" t="inlineStr"/>
-      <c r="O57" t="inlineStr"/>
-      <c r="P57" t="inlineStr"/>
+      <c r="L57" t="n">
+        <v>0</v>
+      </c>
+      <c r="M57" t="n">
+        <v>0</v>
+      </c>
+      <c r="N57" t="n">
+        <v>0</v>
+      </c>
+      <c r="O57" t="n">
+        <v>0</v>
+      </c>
+      <c r="P57" t="n">
+        <v>0</v>
+      </c>
       <c r="Q57" t="n">
         <v>0</v>
       </c>
@@ -3562,15 +4200,27 @@
       <c r="I58" t="n">
         <v>2</v>
       </c>
-      <c r="J58" t="inlineStr"/>
-      <c r="K58" t="inlineStr"/>
+      <c r="J58" t="n">
+        <v>0</v>
+      </c>
+      <c r="K58" t="n">
+        <v>0</v>
+      </c>
       <c r="L58" t="n">
         <v>9</v>
       </c>
-      <c r="M58" t="inlineStr"/>
-      <c r="N58" t="inlineStr"/>
-      <c r="O58" t="inlineStr"/>
-      <c r="P58" t="inlineStr"/>
+      <c r="M58" t="n">
+        <v>0</v>
+      </c>
+      <c r="N58" t="n">
+        <v>0</v>
+      </c>
+      <c r="O58" t="n">
+        <v>0</v>
+      </c>
+      <c r="P58" t="n">
+        <v>0</v>
+      </c>
       <c r="Q58" t="n">
         <v>3</v>
       </c>
@@ -3615,15 +4265,27 @@
       <c r="I59" t="n">
         <v>4</v>
       </c>
-      <c r="J59" t="inlineStr"/>
-      <c r="K59" t="inlineStr"/>
+      <c r="J59" t="n">
+        <v>0</v>
+      </c>
+      <c r="K59" t="n">
+        <v>0</v>
+      </c>
       <c r="L59" t="n">
         <v>8</v>
       </c>
-      <c r="M59" t="inlineStr"/>
-      <c r="N59" t="inlineStr"/>
-      <c r="O59" t="inlineStr"/>
-      <c r="P59" t="inlineStr"/>
+      <c r="M59" t="n">
+        <v>0</v>
+      </c>
+      <c r="N59" t="n">
+        <v>0</v>
+      </c>
+      <c r="O59" t="n">
+        <v>0</v>
+      </c>
+      <c r="P59" t="n">
+        <v>0</v>
+      </c>
       <c r="Q59" t="n">
         <v>0</v>
       </c>
@@ -3668,17 +4330,27 @@
       <c r="I60" t="n">
         <v>34</v>
       </c>
-      <c r="J60" t="inlineStr"/>
+      <c r="J60" t="n">
+        <v>0</v>
+      </c>
       <c r="K60" t="n">
         <v>57</v>
       </c>
       <c r="L60" t="n">
         <v>2</v>
       </c>
-      <c r="M60" t="inlineStr"/>
-      <c r="N60" t="inlineStr"/>
-      <c r="O60" t="inlineStr"/>
-      <c r="P60" t="inlineStr"/>
+      <c r="M60" t="n">
+        <v>0</v>
+      </c>
+      <c r="N60" t="n">
+        <v>0</v>
+      </c>
+      <c r="O60" t="n">
+        <v>0</v>
+      </c>
+      <c r="P60" t="n">
+        <v>0</v>
+      </c>
       <c r="Q60" t="n">
         <v>2</v>
       </c>
@@ -3723,17 +4395,27 @@
       <c r="I61" t="n">
         <v>57</v>
       </c>
-      <c r="J61" t="inlineStr"/>
+      <c r="J61" t="n">
+        <v>0</v>
+      </c>
       <c r="K61" t="n">
         <v>88</v>
       </c>
       <c r="L61" t="n">
         <v>2</v>
       </c>
-      <c r="M61" t="inlineStr"/>
-      <c r="N61" t="inlineStr"/>
-      <c r="O61" t="inlineStr"/>
-      <c r="P61" t="inlineStr"/>
+      <c r="M61" t="n">
+        <v>0</v>
+      </c>
+      <c r="N61" t="n">
+        <v>0</v>
+      </c>
+      <c r="O61" t="n">
+        <v>0</v>
+      </c>
+      <c r="P61" t="n">
+        <v>0</v>
+      </c>
       <c r="Q61" t="n">
         <v>4</v>
       </c>
@@ -3778,15 +4460,27 @@
       <c r="I62" t="n">
         <v>18</v>
       </c>
-      <c r="J62" t="inlineStr"/>
+      <c r="J62" t="n">
+        <v>0</v>
+      </c>
       <c r="K62" t="n">
         <v>32</v>
       </c>
-      <c r="L62" t="inlineStr"/>
-      <c r="M62" t="inlineStr"/>
-      <c r="N62" t="inlineStr"/>
-      <c r="O62" t="inlineStr"/>
-      <c r="P62" t="inlineStr"/>
+      <c r="L62" t="n">
+        <v>0</v>
+      </c>
+      <c r="M62" t="n">
+        <v>0</v>
+      </c>
+      <c r="N62" t="n">
+        <v>0</v>
+      </c>
+      <c r="O62" t="n">
+        <v>0</v>
+      </c>
+      <c r="P62" t="n">
+        <v>0</v>
+      </c>
       <c r="Q62" t="n">
         <v>4</v>
       </c>
@@ -3831,17 +4525,27 @@
       <c r="I63" t="n">
         <v>31</v>
       </c>
-      <c r="J63" t="inlineStr"/>
+      <c r="J63" t="n">
+        <v>0</v>
+      </c>
       <c r="K63" t="n">
         <v>57</v>
       </c>
       <c r="L63" t="n">
         <v>3</v>
       </c>
-      <c r="M63" t="inlineStr"/>
-      <c r="N63" t="inlineStr"/>
-      <c r="O63" t="inlineStr"/>
-      <c r="P63" t="inlineStr"/>
+      <c r="M63" t="n">
+        <v>0</v>
+      </c>
+      <c r="N63" t="n">
+        <v>0</v>
+      </c>
+      <c r="O63" t="n">
+        <v>0</v>
+      </c>
+      <c r="P63" t="n">
+        <v>0</v>
+      </c>
       <c r="Q63" t="n">
         <v>2</v>
       </c>
@@ -3886,15 +4590,27 @@
       <c r="I64" t="n">
         <v>9</v>
       </c>
-      <c r="J64" t="inlineStr"/>
-      <c r="K64" t="inlineStr"/>
+      <c r="J64" t="n">
+        <v>0</v>
+      </c>
+      <c r="K64" t="n">
+        <v>0</v>
+      </c>
       <c r="L64" t="n">
         <v>16</v>
       </c>
-      <c r="M64" t="inlineStr"/>
-      <c r="N64" t="inlineStr"/>
-      <c r="O64" t="inlineStr"/>
-      <c r="P64" t="inlineStr"/>
+      <c r="M64" t="n">
+        <v>0</v>
+      </c>
+      <c r="N64" t="n">
+        <v>0</v>
+      </c>
+      <c r="O64" t="n">
+        <v>0</v>
+      </c>
+      <c r="P64" t="n">
+        <v>0</v>
+      </c>
       <c r="Q64" t="n">
         <v>0</v>
       </c>
@@ -3939,15 +4655,27 @@
       <c r="I65" t="n">
         <v>50</v>
       </c>
-      <c r="J65" t="inlineStr"/>
+      <c r="J65" t="n">
+        <v>0</v>
+      </c>
       <c r="K65" t="n">
         <v>82</v>
       </c>
-      <c r="L65" t="inlineStr"/>
-      <c r="M65" t="inlineStr"/>
-      <c r="N65" t="inlineStr"/>
-      <c r="O65" t="inlineStr"/>
-      <c r="P65" t="inlineStr"/>
+      <c r="L65" t="n">
+        <v>0</v>
+      </c>
+      <c r="M65" t="n">
+        <v>0</v>
+      </c>
+      <c r="N65" t="n">
+        <v>0</v>
+      </c>
+      <c r="O65" t="n">
+        <v>0</v>
+      </c>
+      <c r="P65" t="n">
+        <v>0</v>
+      </c>
       <c r="Q65" t="n">
         <v>8</v>
       </c>
@@ -4004,8 +4732,12 @@
       <c r="M66" t="n">
         <v>5</v>
       </c>
-      <c r="N66" t="inlineStr"/>
-      <c r="O66" t="inlineStr"/>
+      <c r="N66" t="n">
+        <v>0</v>
+      </c>
+      <c r="O66" t="n">
+        <v>0</v>
+      </c>
       <c r="P66" t="n">
         <v>1</v>
       </c>
@@ -4065,9 +4797,15 @@
       <c r="M67" t="n">
         <v>14</v>
       </c>
-      <c r="N67" t="inlineStr"/>
-      <c r="O67" t="inlineStr"/>
-      <c r="P67" t="inlineStr"/>
+      <c r="N67" t="n">
+        <v>0</v>
+      </c>
+      <c r="O67" t="n">
+        <v>0</v>
+      </c>
+      <c r="P67" t="n">
+        <v>0</v>
+      </c>
       <c r="Q67" t="n">
         <v>6</v>
       </c>
@@ -4115,14 +4853,24 @@
       <c r="J68" t="n">
         <v>3</v>
       </c>
-      <c r="K68" t="inlineStr"/>
+      <c r="K68" t="n">
+        <v>0</v>
+      </c>
       <c r="L68" t="n">
         <v>17</v>
       </c>
-      <c r="M68" t="inlineStr"/>
-      <c r="N68" t="inlineStr"/>
-      <c r="O68" t="inlineStr"/>
-      <c r="P68" t="inlineStr"/>
+      <c r="M68" t="n">
+        <v>0</v>
+      </c>
+      <c r="N68" t="n">
+        <v>0</v>
+      </c>
+      <c r="O68" t="n">
+        <v>0</v>
+      </c>
+      <c r="P68" t="n">
+        <v>0</v>
+      </c>
       <c r="Q68" t="n">
         <v>3</v>
       </c>
@@ -4167,17 +4915,27 @@
       <c r="I69" t="n">
         <v>21</v>
       </c>
-      <c r="J69" t="inlineStr"/>
+      <c r="J69" t="n">
+        <v>0</v>
+      </c>
       <c r="K69" t="n">
         <v>3</v>
       </c>
       <c r="L69" t="n">
         <v>33</v>
       </c>
-      <c r="M69" t="inlineStr"/>
-      <c r="N69" t="inlineStr"/>
-      <c r="O69" t="inlineStr"/>
-      <c r="P69" t="inlineStr"/>
+      <c r="M69" t="n">
+        <v>0</v>
+      </c>
+      <c r="N69" t="n">
+        <v>0</v>
+      </c>
+      <c r="O69" t="n">
+        <v>0</v>
+      </c>
+      <c r="P69" t="n">
+        <v>0</v>
+      </c>
       <c r="Q69" t="n">
         <v>2</v>
       </c>
@@ -4222,17 +4980,27 @@
       <c r="I70" t="n">
         <v>36</v>
       </c>
-      <c r="J70" t="inlineStr"/>
+      <c r="J70" t="n">
+        <v>0</v>
+      </c>
       <c r="K70" t="n">
         <v>48</v>
       </c>
       <c r="L70" t="n">
         <v>5</v>
       </c>
-      <c r="M70" t="inlineStr"/>
-      <c r="N70" t="inlineStr"/>
-      <c r="O70" t="inlineStr"/>
-      <c r="P70" t="inlineStr"/>
+      <c r="M70" t="n">
+        <v>0</v>
+      </c>
+      <c r="N70" t="n">
+        <v>0</v>
+      </c>
+      <c r="O70" t="n">
+        <v>0</v>
+      </c>
+      <c r="P70" t="n">
+        <v>0</v>
+      </c>
       <c r="Q70" t="n">
         <v>2</v>
       </c>
@@ -4277,15 +5045,27 @@
       <c r="I71" t="n">
         <v>17</v>
       </c>
-      <c r="J71" t="inlineStr"/>
+      <c r="J71" t="n">
+        <v>0</v>
+      </c>
       <c r="K71" t="n">
         <v>26</v>
       </c>
-      <c r="L71" t="inlineStr"/>
-      <c r="M71" t="inlineStr"/>
-      <c r="N71" t="inlineStr"/>
-      <c r="O71" t="inlineStr"/>
-      <c r="P71" t="inlineStr"/>
+      <c r="L71" t="n">
+        <v>0</v>
+      </c>
+      <c r="M71" t="n">
+        <v>0</v>
+      </c>
+      <c r="N71" t="n">
+        <v>0</v>
+      </c>
+      <c r="O71" t="n">
+        <v>0</v>
+      </c>
+      <c r="P71" t="n">
+        <v>0</v>
+      </c>
       <c r="Q71" t="n">
         <v>1</v>
       </c>
@@ -4330,17 +5110,27 @@
       <c r="I72" t="n">
         <v>11</v>
       </c>
-      <c r="J72" t="inlineStr"/>
+      <c r="J72" t="n">
+        <v>0</v>
+      </c>
       <c r="K72" t="n">
         <v>20</v>
       </c>
       <c r="L72" t="n">
         <v>3</v>
       </c>
-      <c r="M72" t="inlineStr"/>
-      <c r="N72" t="inlineStr"/>
-      <c r="O72" t="inlineStr"/>
-      <c r="P72" t="inlineStr"/>
+      <c r="M72" t="n">
+        <v>0</v>
+      </c>
+      <c r="N72" t="n">
+        <v>0</v>
+      </c>
+      <c r="O72" t="n">
+        <v>0</v>
+      </c>
+      <c r="P72" t="n">
+        <v>0</v>
+      </c>
       <c r="Q72" t="n">
         <v>2</v>
       </c>
@@ -4385,15 +5175,27 @@
       <c r="I73" t="n">
         <v>37</v>
       </c>
-      <c r="J73" t="inlineStr"/>
+      <c r="J73" t="n">
+        <v>0</v>
+      </c>
       <c r="K73" t="n">
         <v>61</v>
       </c>
-      <c r="L73" t="inlineStr"/>
-      <c r="M73" t="inlineStr"/>
-      <c r="N73" t="inlineStr"/>
-      <c r="O73" t="inlineStr"/>
-      <c r="P73" t="inlineStr"/>
+      <c r="L73" t="n">
+        <v>0</v>
+      </c>
+      <c r="M73" t="n">
+        <v>0</v>
+      </c>
+      <c r="N73" t="n">
+        <v>0</v>
+      </c>
+      <c r="O73" t="n">
+        <v>0</v>
+      </c>
+      <c r="P73" t="n">
+        <v>0</v>
+      </c>
       <c r="Q73" t="n">
         <v>3</v>
       </c>
@@ -4441,14 +5243,24 @@
       <c r="J74" t="n">
         <v>3</v>
       </c>
-      <c r="K74" t="inlineStr"/>
+      <c r="K74" t="n">
+        <v>0</v>
+      </c>
       <c r="L74" t="n">
         <v>41</v>
       </c>
-      <c r="M74" t="inlineStr"/>
-      <c r="N74" t="inlineStr"/>
-      <c r="O74" t="inlineStr"/>
-      <c r="P74" t="inlineStr"/>
+      <c r="M74" t="n">
+        <v>0</v>
+      </c>
+      <c r="N74" t="n">
+        <v>0</v>
+      </c>
+      <c r="O74" t="n">
+        <v>0</v>
+      </c>
+      <c r="P74" t="n">
+        <v>0</v>
+      </c>
       <c r="Q74" t="n">
         <v>5</v>
       </c>
@@ -4493,16 +5305,24 @@
       <c r="I75" t="n">
         <v>53</v>
       </c>
-      <c r="J75" t="inlineStr"/>
+      <c r="J75" t="n">
+        <v>0</v>
+      </c>
       <c r="K75" t="n">
         <v>24</v>
       </c>
       <c r="L75" t="n">
         <v>61</v>
       </c>
-      <c r="M75" t="inlineStr"/>
-      <c r="N75" t="inlineStr"/>
-      <c r="O75" t="inlineStr"/>
+      <c r="M75" t="n">
+        <v>0</v>
+      </c>
+      <c r="N75" t="n">
+        <v>0</v>
+      </c>
+      <c r="O75" t="n">
+        <v>0</v>
+      </c>
       <c r="P75" t="n">
         <v>2</v>
       </c>
@@ -4550,17 +5370,27 @@
       <c r="I76" t="n">
         <v>52</v>
       </c>
-      <c r="J76" t="inlineStr"/>
+      <c r="J76" t="n">
+        <v>0</v>
+      </c>
       <c r="K76" t="n">
         <v>40</v>
       </c>
       <c r="L76" t="n">
         <v>39</v>
       </c>
-      <c r="M76" t="inlineStr"/>
-      <c r="N76" t="inlineStr"/>
-      <c r="O76" t="inlineStr"/>
-      <c r="P76" t="inlineStr"/>
+      <c r="M76" t="n">
+        <v>0</v>
+      </c>
+      <c r="N76" t="n">
+        <v>0</v>
+      </c>
+      <c r="O76" t="n">
+        <v>0</v>
+      </c>
+      <c r="P76" t="n">
+        <v>0</v>
+      </c>
       <c r="Q76" t="n">
         <v>8</v>
       </c>
@@ -4605,17 +5435,27 @@
       <c r="I77" t="n">
         <v>15</v>
       </c>
-      <c r="J77" t="inlineStr"/>
+      <c r="J77" t="n">
+        <v>0</v>
+      </c>
       <c r="K77" t="n">
         <v>18</v>
       </c>
       <c r="L77" t="n">
         <v>4</v>
       </c>
-      <c r="M77" t="inlineStr"/>
-      <c r="N77" t="inlineStr"/>
-      <c r="O77" t="inlineStr"/>
-      <c r="P77" t="inlineStr"/>
+      <c r="M77" t="n">
+        <v>0</v>
+      </c>
+      <c r="N77" t="n">
+        <v>0</v>
+      </c>
+      <c r="O77" t="n">
+        <v>0</v>
+      </c>
+      <c r="P77" t="n">
+        <v>0</v>
+      </c>
       <c r="Q77" t="n">
         <v>3</v>
       </c>
@@ -4660,15 +5500,27 @@
       <c r="I78" t="n">
         <v>35</v>
       </c>
-      <c r="J78" t="inlineStr"/>
-      <c r="K78" t="inlineStr"/>
+      <c r="J78" t="n">
+        <v>0</v>
+      </c>
+      <c r="K78" t="n">
+        <v>0</v>
+      </c>
       <c r="L78" t="n">
         <v>50</v>
       </c>
-      <c r="M78" t="inlineStr"/>
-      <c r="N78" t="inlineStr"/>
-      <c r="O78" t="inlineStr"/>
-      <c r="P78" t="inlineStr"/>
+      <c r="M78" t="n">
+        <v>0</v>
+      </c>
+      <c r="N78" t="n">
+        <v>0</v>
+      </c>
+      <c r="O78" t="n">
+        <v>0</v>
+      </c>
+      <c r="P78" t="n">
+        <v>0</v>
+      </c>
       <c r="Q78" t="n">
         <v>6</v>
       </c>
@@ -4713,15 +5565,27 @@
       <c r="I79" t="n">
         <v>9</v>
       </c>
-      <c r="J79" t="inlineStr"/>
+      <c r="J79" t="n">
+        <v>0</v>
+      </c>
       <c r="K79" t="n">
         <v>18</v>
       </c>
-      <c r="L79" t="inlineStr"/>
-      <c r="M79" t="inlineStr"/>
-      <c r="N79" t="inlineStr"/>
-      <c r="O79" t="inlineStr"/>
-      <c r="P79" t="inlineStr"/>
+      <c r="L79" t="n">
+        <v>0</v>
+      </c>
+      <c r="M79" t="n">
+        <v>0</v>
+      </c>
+      <c r="N79" t="n">
+        <v>0</v>
+      </c>
+      <c r="O79" t="n">
+        <v>0</v>
+      </c>
+      <c r="P79" t="n">
+        <v>0</v>
+      </c>
       <c r="Q79" t="n">
         <v>1</v>
       </c>
@@ -4766,17 +5630,27 @@
       <c r="I80" t="n">
         <v>65</v>
       </c>
-      <c r="J80" t="inlineStr"/>
+      <c r="J80" t="n">
+        <v>0</v>
+      </c>
       <c r="K80" t="n">
         <v>22</v>
       </c>
       <c r="L80" t="n">
         <v>77</v>
       </c>
-      <c r="M80" t="inlineStr"/>
-      <c r="N80" t="inlineStr"/>
-      <c r="O80" t="inlineStr"/>
-      <c r="P80" t="inlineStr"/>
+      <c r="M80" t="n">
+        <v>0</v>
+      </c>
+      <c r="N80" t="n">
+        <v>0</v>
+      </c>
+      <c r="O80" t="n">
+        <v>0</v>
+      </c>
+      <c r="P80" t="n">
+        <v>0</v>
+      </c>
       <c r="Q80" t="n">
         <v>12</v>
       </c>
@@ -4821,17 +5695,27 @@
       <c r="I81" t="n">
         <v>67</v>
       </c>
-      <c r="J81" t="inlineStr"/>
+      <c r="J81" t="n">
+        <v>0</v>
+      </c>
       <c r="K81" t="n">
         <v>99</v>
       </c>
       <c r="L81" t="n">
         <v>15</v>
       </c>
-      <c r="M81" t="inlineStr"/>
-      <c r="N81" t="inlineStr"/>
-      <c r="O81" t="inlineStr"/>
-      <c r="P81" t="inlineStr"/>
+      <c r="M81" t="n">
+        <v>0</v>
+      </c>
+      <c r="N81" t="n">
+        <v>0</v>
+      </c>
+      <c r="O81" t="n">
+        <v>0</v>
+      </c>
+      <c r="P81" t="n">
+        <v>0</v>
+      </c>
       <c r="Q81" t="n">
         <v>11</v>
       </c>
@@ -4876,17 +5760,27 @@
       <c r="I82" t="n">
         <v>38</v>
       </c>
-      <c r="J82" t="inlineStr"/>
+      <c r="J82" t="n">
+        <v>0</v>
+      </c>
       <c r="K82" t="n">
         <v>70</v>
       </c>
       <c r="L82" t="n">
         <v>5</v>
       </c>
-      <c r="M82" t="inlineStr"/>
-      <c r="N82" t="inlineStr"/>
-      <c r="O82" t="inlineStr"/>
-      <c r="P82" t="inlineStr"/>
+      <c r="M82" t="n">
+        <v>0</v>
+      </c>
+      <c r="N82" t="n">
+        <v>0</v>
+      </c>
+      <c r="O82" t="n">
+        <v>0</v>
+      </c>
+      <c r="P82" t="n">
+        <v>0</v>
+      </c>
       <c r="Q82" t="n">
         <v>5</v>
       </c>
@@ -4931,17 +5825,27 @@
       <c r="I83" t="n">
         <v>67</v>
       </c>
-      <c r="J83" t="inlineStr"/>
+      <c r="J83" t="n">
+        <v>0</v>
+      </c>
       <c r="K83" t="n">
         <v>75</v>
       </c>
       <c r="L83" t="n">
         <v>58</v>
       </c>
-      <c r="M83" t="inlineStr"/>
-      <c r="N83" t="inlineStr"/>
-      <c r="O83" t="inlineStr"/>
-      <c r="P83" t="inlineStr"/>
+      <c r="M83" t="n">
+        <v>0</v>
+      </c>
+      <c r="N83" t="n">
+        <v>0</v>
+      </c>
+      <c r="O83" t="n">
+        <v>0</v>
+      </c>
+      <c r="P83" t="n">
+        <v>0</v>
+      </c>
       <c r="Q83" t="n">
         <v>13</v>
       </c>
@@ -4995,10 +5899,18 @@
       <c r="L84" t="n">
         <v>46</v>
       </c>
-      <c r="M84" t="inlineStr"/>
-      <c r="N84" t="inlineStr"/>
-      <c r="O84" t="inlineStr"/>
-      <c r="P84" t="inlineStr"/>
+      <c r="M84" t="n">
+        <v>0</v>
+      </c>
+      <c r="N84" t="n">
+        <v>0</v>
+      </c>
+      <c r="O84" t="n">
+        <v>0</v>
+      </c>
+      <c r="P84" t="n">
+        <v>0</v>
+      </c>
       <c r="Q84" t="n">
         <v>6</v>
       </c>
@@ -5043,15 +5955,27 @@
       <c r="I85" t="n">
         <v>59</v>
       </c>
-      <c r="J85" t="inlineStr"/>
+      <c r="J85" t="n">
+        <v>0</v>
+      </c>
       <c r="K85" t="n">
         <v>97</v>
       </c>
-      <c r="L85" t="inlineStr"/>
-      <c r="M85" t="inlineStr"/>
-      <c r="N85" t="inlineStr"/>
-      <c r="O85" t="inlineStr"/>
-      <c r="P85" t="inlineStr"/>
+      <c r="L85" t="n">
+        <v>0</v>
+      </c>
+      <c r="M85" t="n">
+        <v>0</v>
+      </c>
+      <c r="N85" t="n">
+        <v>0</v>
+      </c>
+      <c r="O85" t="n">
+        <v>0</v>
+      </c>
+      <c r="P85" t="n">
+        <v>0</v>
+      </c>
       <c r="Q85" t="n">
         <v>5</v>
       </c>
@@ -5096,17 +6020,27 @@
       <c r="I86" t="n">
         <v>27</v>
       </c>
-      <c r="J86" t="inlineStr"/>
+      <c r="J86" t="n">
+        <v>0</v>
+      </c>
       <c r="K86" t="n">
         <v>24</v>
       </c>
       <c r="L86" t="n">
         <v>14</v>
       </c>
-      <c r="M86" t="inlineStr"/>
-      <c r="N86" t="inlineStr"/>
-      <c r="O86" t="inlineStr"/>
-      <c r="P86" t="inlineStr"/>
+      <c r="M86" t="n">
+        <v>0</v>
+      </c>
+      <c r="N86" t="n">
+        <v>0</v>
+      </c>
+      <c r="O86" t="n">
+        <v>0</v>
+      </c>
+      <c r="P86" t="n">
+        <v>0</v>
+      </c>
       <c r="Q86" t="n">
         <v>2</v>
       </c>
@@ -5151,15 +6085,27 @@
       <c r="I87" t="n">
         <v>51</v>
       </c>
-      <c r="J87" t="inlineStr"/>
+      <c r="J87" t="n">
+        <v>0</v>
+      </c>
       <c r="K87" t="n">
         <v>92</v>
       </c>
-      <c r="L87" t="inlineStr"/>
-      <c r="M87" t="inlineStr"/>
-      <c r="N87" t="inlineStr"/>
-      <c r="O87" t="inlineStr"/>
-      <c r="P87" t="inlineStr"/>
+      <c r="L87" t="n">
+        <v>0</v>
+      </c>
+      <c r="M87" t="n">
+        <v>0</v>
+      </c>
+      <c r="N87" t="n">
+        <v>0</v>
+      </c>
+      <c r="O87" t="n">
+        <v>0</v>
+      </c>
+      <c r="P87" t="n">
+        <v>0</v>
+      </c>
       <c r="Q87" t="n">
         <v>4</v>
       </c>
@@ -5204,17 +6150,27 @@
       <c r="I88" t="n">
         <v>29</v>
       </c>
-      <c r="J88" t="inlineStr"/>
+      <c r="J88" t="n">
+        <v>0</v>
+      </c>
       <c r="K88" t="n">
         <v>0</v>
       </c>
       <c r="L88" t="n">
         <v>55</v>
       </c>
-      <c r="M88" t="inlineStr"/>
-      <c r="N88" t="inlineStr"/>
-      <c r="O88" t="inlineStr"/>
-      <c r="P88" t="inlineStr"/>
+      <c r="M88" t="n">
+        <v>0</v>
+      </c>
+      <c r="N88" t="n">
+        <v>0</v>
+      </c>
+      <c r="O88" t="n">
+        <v>0</v>
+      </c>
+      <c r="P88" t="n">
+        <v>0</v>
+      </c>
       <c r="Q88" t="n">
         <v>3</v>
       </c>
@@ -5259,15 +6215,27 @@
       <c r="I89" t="n">
         <v>54</v>
       </c>
-      <c r="J89" t="inlineStr"/>
+      <c r="J89" t="n">
+        <v>0</v>
+      </c>
       <c r="K89" t="n">
         <v>106</v>
       </c>
-      <c r="L89" t="inlineStr"/>
-      <c r="M89" t="inlineStr"/>
-      <c r="N89" t="inlineStr"/>
-      <c r="O89" t="inlineStr"/>
-      <c r="P89" t="inlineStr"/>
+      <c r="L89" t="n">
+        <v>0</v>
+      </c>
+      <c r="M89" t="n">
+        <v>0</v>
+      </c>
+      <c r="N89" t="n">
+        <v>0</v>
+      </c>
+      <c r="O89" t="n">
+        <v>0</v>
+      </c>
+      <c r="P89" t="n">
+        <v>0</v>
+      </c>
       <c r="Q89" t="n">
         <v>5</v>
       </c>
@@ -5324,9 +6292,15 @@
       <c r="M90" t="n">
         <v>11</v>
       </c>
-      <c r="N90" t="inlineStr"/>
-      <c r="O90" t="inlineStr"/>
-      <c r="P90" t="inlineStr"/>
+      <c r="N90" t="n">
+        <v>0</v>
+      </c>
+      <c r="O90" t="n">
+        <v>0</v>
+      </c>
+      <c r="P90" t="n">
+        <v>0</v>
+      </c>
       <c r="Q90" t="n">
         <v>10</v>
       </c>
@@ -5362,17 +6336,39 @@
           <t>CHARTER SCH</t>
         </is>
       </c>
-      <c r="G91" t="inlineStr"/>
-      <c r="H91" t="inlineStr"/>
-      <c r="I91" t="inlineStr"/>
-      <c r="J91" t="inlineStr"/>
-      <c r="K91" t="inlineStr"/>
-      <c r="L91" t="inlineStr"/>
-      <c r="M91" t="inlineStr"/>
-      <c r="N91" t="inlineStr"/>
-      <c r="O91" t="inlineStr"/>
-      <c r="P91" t="inlineStr"/>
-      <c r="Q91" t="inlineStr"/>
+      <c r="G91" t="n">
+        <v>0</v>
+      </c>
+      <c r="H91" t="n">
+        <v>0</v>
+      </c>
+      <c r="I91" t="n">
+        <v>0</v>
+      </c>
+      <c r="J91" t="n">
+        <v>0</v>
+      </c>
+      <c r="K91" t="n">
+        <v>0</v>
+      </c>
+      <c r="L91" t="n">
+        <v>0</v>
+      </c>
+      <c r="M91" t="n">
+        <v>0</v>
+      </c>
+      <c r="N91" t="n">
+        <v>0</v>
+      </c>
+      <c r="O91" t="n">
+        <v>0</v>
+      </c>
+      <c r="P91" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q91" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -5414,15 +6410,27 @@
       <c r="I92" t="n">
         <v>20</v>
       </c>
-      <c r="J92" t="inlineStr"/>
+      <c r="J92" t="n">
+        <v>0</v>
+      </c>
       <c r="K92" t="n">
         <v>30</v>
       </c>
-      <c r="L92" t="inlineStr"/>
-      <c r="M92" t="inlineStr"/>
-      <c r="N92" t="inlineStr"/>
-      <c r="O92" t="inlineStr"/>
-      <c r="P92" t="inlineStr"/>
+      <c r="L92" t="n">
+        <v>0</v>
+      </c>
+      <c r="M92" t="n">
+        <v>0</v>
+      </c>
+      <c r="N92" t="n">
+        <v>0</v>
+      </c>
+      <c r="O92" t="n">
+        <v>0</v>
+      </c>
+      <c r="P92" t="n">
+        <v>0</v>
+      </c>
       <c r="Q92" t="n">
         <v>0</v>
       </c>
@@ -5467,15 +6475,27 @@
       <c r="I93" t="n">
         <v>3</v>
       </c>
-      <c r="J93" t="inlineStr"/>
-      <c r="K93" t="inlineStr"/>
+      <c r="J93" t="n">
+        <v>0</v>
+      </c>
+      <c r="K93" t="n">
+        <v>0</v>
+      </c>
       <c r="L93" t="n">
         <v>11</v>
       </c>
-      <c r="M93" t="inlineStr"/>
-      <c r="N93" t="inlineStr"/>
-      <c r="O93" t="inlineStr"/>
-      <c r="P93" t="inlineStr"/>
+      <c r="M93" t="n">
+        <v>0</v>
+      </c>
+      <c r="N93" t="n">
+        <v>0</v>
+      </c>
+      <c r="O93" t="n">
+        <v>0</v>
+      </c>
+      <c r="P93" t="n">
+        <v>0</v>
+      </c>
       <c r="Q93" t="n">
         <v>2</v>
       </c>
@@ -5520,15 +6540,27 @@
       <c r="I94" t="n">
         <v>31</v>
       </c>
-      <c r="J94" t="inlineStr"/>
-      <c r="K94" t="inlineStr"/>
+      <c r="J94" t="n">
+        <v>0</v>
+      </c>
+      <c r="K94" t="n">
+        <v>0</v>
+      </c>
       <c r="L94" t="n">
         <v>61</v>
       </c>
-      <c r="M94" t="inlineStr"/>
-      <c r="N94" t="inlineStr"/>
-      <c r="O94" t="inlineStr"/>
-      <c r="P94" t="inlineStr"/>
+      <c r="M94" t="n">
+        <v>0</v>
+      </c>
+      <c r="N94" t="n">
+        <v>0</v>
+      </c>
+      <c r="O94" t="n">
+        <v>0</v>
+      </c>
+      <c r="P94" t="n">
+        <v>0</v>
+      </c>
       <c r="Q94" t="n">
         <v>12</v>
       </c>
@@ -5573,15 +6605,27 @@
       <c r="I95" t="n">
         <v>30</v>
       </c>
-      <c r="J95" t="inlineStr"/>
-      <c r="K95" t="inlineStr"/>
+      <c r="J95" t="n">
+        <v>0</v>
+      </c>
+      <c r="K95" t="n">
+        <v>0</v>
+      </c>
       <c r="L95" t="n">
         <v>46</v>
       </c>
-      <c r="M95" t="inlineStr"/>
-      <c r="N95" t="inlineStr"/>
-      <c r="O95" t="inlineStr"/>
-      <c r="P95" t="inlineStr"/>
+      <c r="M95" t="n">
+        <v>0</v>
+      </c>
+      <c r="N95" t="n">
+        <v>0</v>
+      </c>
+      <c r="O95" t="n">
+        <v>0</v>
+      </c>
+      <c r="P95" t="n">
+        <v>0</v>
+      </c>
       <c r="Q95" t="n">
         <v>5</v>
       </c>
@@ -5626,15 +6670,27 @@
       <c r="I96" t="n">
         <v>18</v>
       </c>
-      <c r="J96" t="inlineStr"/>
-      <c r="K96" t="inlineStr"/>
+      <c r="J96" t="n">
+        <v>0</v>
+      </c>
+      <c r="K96" t="n">
+        <v>0</v>
+      </c>
       <c r="L96" t="n">
         <v>27</v>
       </c>
-      <c r="M96" t="inlineStr"/>
-      <c r="N96" t="inlineStr"/>
-      <c r="O96" t="inlineStr"/>
-      <c r="P96" t="inlineStr"/>
+      <c r="M96" t="n">
+        <v>0</v>
+      </c>
+      <c r="N96" t="n">
+        <v>0</v>
+      </c>
+      <c r="O96" t="n">
+        <v>0</v>
+      </c>
+      <c r="P96" t="n">
+        <v>0</v>
+      </c>
       <c r="Q96" t="n">
         <v>1</v>
       </c>
@@ -5679,15 +6735,27 @@
       <c r="I97" t="n">
         <v>31</v>
       </c>
-      <c r="J97" t="inlineStr"/>
-      <c r="K97" t="inlineStr"/>
+      <c r="J97" t="n">
+        <v>0</v>
+      </c>
+      <c r="K97" t="n">
+        <v>0</v>
+      </c>
       <c r="L97" t="n">
         <v>49</v>
       </c>
-      <c r="M97" t="inlineStr"/>
-      <c r="N97" t="inlineStr"/>
-      <c r="O97" t="inlineStr"/>
-      <c r="P97" t="inlineStr"/>
+      <c r="M97" t="n">
+        <v>0</v>
+      </c>
+      <c r="N97" t="n">
+        <v>0</v>
+      </c>
+      <c r="O97" t="n">
+        <v>0</v>
+      </c>
+      <c r="P97" t="n">
+        <v>0</v>
+      </c>
       <c r="Q97" t="n">
         <v>2</v>
       </c>
@@ -5732,15 +6800,27 @@
       <c r="I98" t="n">
         <v>38</v>
       </c>
-      <c r="J98" t="inlineStr"/>
-      <c r="K98" t="inlineStr"/>
+      <c r="J98" t="n">
+        <v>0</v>
+      </c>
+      <c r="K98" t="n">
+        <v>0</v>
+      </c>
       <c r="L98" t="n">
         <v>57</v>
       </c>
-      <c r="M98" t="inlineStr"/>
-      <c r="N98" t="inlineStr"/>
-      <c r="O98" t="inlineStr"/>
-      <c r="P98" t="inlineStr"/>
+      <c r="M98" t="n">
+        <v>0</v>
+      </c>
+      <c r="N98" t="n">
+        <v>0</v>
+      </c>
+      <c r="O98" t="n">
+        <v>0</v>
+      </c>
+      <c r="P98" t="n">
+        <v>0</v>
+      </c>
       <c r="Q98" t="n">
         <v>4</v>
       </c>
@@ -5785,15 +6865,27 @@
       <c r="I99" t="n">
         <v>30</v>
       </c>
-      <c r="J99" t="inlineStr"/>
-      <c r="K99" t="inlineStr"/>
+      <c r="J99" t="n">
+        <v>0</v>
+      </c>
+      <c r="K99" t="n">
+        <v>0</v>
+      </c>
       <c r="L99" t="n">
         <v>41</v>
       </c>
-      <c r="M99" t="inlineStr"/>
-      <c r="N99" t="inlineStr"/>
-      <c r="O99" t="inlineStr"/>
-      <c r="P99" t="inlineStr"/>
+      <c r="M99" t="n">
+        <v>0</v>
+      </c>
+      <c r="N99" t="n">
+        <v>0</v>
+      </c>
+      <c r="O99" t="n">
+        <v>0</v>
+      </c>
+      <c r="P99" t="n">
+        <v>0</v>
+      </c>
       <c r="Q99" t="n">
         <v>4</v>
       </c>
@@ -5838,15 +6930,27 @@
       <c r="I100" t="n">
         <v>21</v>
       </c>
-      <c r="J100" t="inlineStr"/>
-      <c r="K100" t="inlineStr"/>
+      <c r="J100" t="n">
+        <v>0</v>
+      </c>
+      <c r="K100" t="n">
+        <v>0</v>
+      </c>
       <c r="L100" t="n">
         <v>34</v>
       </c>
-      <c r="M100" t="inlineStr"/>
-      <c r="N100" t="inlineStr"/>
-      <c r="O100" t="inlineStr"/>
-      <c r="P100" t="inlineStr"/>
+      <c r="M100" t="n">
+        <v>0</v>
+      </c>
+      <c r="N100" t="n">
+        <v>0</v>
+      </c>
+      <c r="O100" t="n">
+        <v>0</v>
+      </c>
+      <c r="P100" t="n">
+        <v>0</v>
+      </c>
       <c r="Q100" t="n">
         <v>3</v>
       </c>
@@ -5891,17 +6995,27 @@
       <c r="I101" t="n">
         <v>16</v>
       </c>
-      <c r="J101" t="inlineStr"/>
+      <c r="J101" t="n">
+        <v>0</v>
+      </c>
       <c r="K101" t="n">
         <v>0</v>
       </c>
       <c r="L101" t="n">
         <v>29</v>
       </c>
-      <c r="M101" t="inlineStr"/>
-      <c r="N101" t="inlineStr"/>
-      <c r="O101" t="inlineStr"/>
-      <c r="P101" t="inlineStr"/>
+      <c r="M101" t="n">
+        <v>0</v>
+      </c>
+      <c r="N101" t="n">
+        <v>0</v>
+      </c>
+      <c r="O101" t="n">
+        <v>0</v>
+      </c>
+      <c r="P101" t="n">
+        <v>0</v>
+      </c>
       <c r="Q101" t="n">
         <v>1</v>
       </c>
@@ -5946,15 +7060,27 @@
       <c r="I102" t="n">
         <v>34</v>
       </c>
-      <c r="J102" t="inlineStr"/>
-      <c r="K102" t="inlineStr"/>
+      <c r="J102" t="n">
+        <v>0</v>
+      </c>
+      <c r="K102" t="n">
+        <v>0</v>
+      </c>
       <c r="L102" t="n">
         <v>64</v>
       </c>
-      <c r="M102" t="inlineStr"/>
-      <c r="N102" t="inlineStr"/>
-      <c r="O102" t="inlineStr"/>
-      <c r="P102" t="inlineStr"/>
+      <c r="M102" t="n">
+        <v>0</v>
+      </c>
+      <c r="N102" t="n">
+        <v>0</v>
+      </c>
+      <c r="O102" t="n">
+        <v>0</v>
+      </c>
+      <c r="P102" t="n">
+        <v>0</v>
+      </c>
       <c r="Q102" t="n">
         <v>4</v>
       </c>
@@ -5999,15 +7125,27 @@
       <c r="I103" t="n">
         <v>37</v>
       </c>
-      <c r="J103" t="inlineStr"/>
+      <c r="J103" t="n">
+        <v>0</v>
+      </c>
       <c r="K103" t="n">
         <v>62</v>
       </c>
-      <c r="L103" t="inlineStr"/>
-      <c r="M103" t="inlineStr"/>
-      <c r="N103" t="inlineStr"/>
-      <c r="O103" t="inlineStr"/>
-      <c r="P103" t="inlineStr"/>
+      <c r="L103" t="n">
+        <v>0</v>
+      </c>
+      <c r="M103" t="n">
+        <v>0</v>
+      </c>
+      <c r="N103" t="n">
+        <v>0</v>
+      </c>
+      <c r="O103" t="n">
+        <v>0</v>
+      </c>
+      <c r="P103" t="n">
+        <v>0</v>
+      </c>
       <c r="Q103" t="n">
         <v>2</v>
       </c>
@@ -6052,15 +7190,27 @@
       <c r="I104" t="n">
         <v>32</v>
       </c>
-      <c r="J104" t="inlineStr"/>
+      <c r="J104" t="n">
+        <v>0</v>
+      </c>
       <c r="K104" t="n">
         <v>43</v>
       </c>
-      <c r="L104" t="inlineStr"/>
-      <c r="M104" t="inlineStr"/>
-      <c r="N104" t="inlineStr"/>
-      <c r="O104" t="inlineStr"/>
-      <c r="P104" t="inlineStr"/>
+      <c r="L104" t="n">
+        <v>0</v>
+      </c>
+      <c r="M104" t="n">
+        <v>0</v>
+      </c>
+      <c r="N104" t="n">
+        <v>0</v>
+      </c>
+      <c r="O104" t="n">
+        <v>0</v>
+      </c>
+      <c r="P104" t="n">
+        <v>0</v>
+      </c>
       <c r="Q104" t="n">
         <v>1</v>
       </c>
@@ -6105,17 +7255,27 @@
       <c r="I105" t="n">
         <v>23</v>
       </c>
-      <c r="J105" t="inlineStr"/>
+      <c r="J105" t="n">
+        <v>0</v>
+      </c>
       <c r="K105" t="n">
         <v>45</v>
       </c>
       <c r="L105" t="n">
         <v>4</v>
       </c>
-      <c r="M105" t="inlineStr"/>
-      <c r="N105" t="inlineStr"/>
-      <c r="O105" t="inlineStr"/>
-      <c r="P105" t="inlineStr"/>
+      <c r="M105" t="n">
+        <v>0</v>
+      </c>
+      <c r="N105" t="n">
+        <v>0</v>
+      </c>
+      <c r="O105" t="n">
+        <v>0</v>
+      </c>
+      <c r="P105" t="n">
+        <v>0</v>
+      </c>
       <c r="Q105" t="n">
         <v>1</v>
       </c>
@@ -6160,15 +7320,27 @@
       <c r="I106" t="n">
         <v>63</v>
       </c>
-      <c r="J106" t="inlineStr"/>
+      <c r="J106" t="n">
+        <v>0</v>
+      </c>
       <c r="K106" t="n">
         <v>103</v>
       </c>
-      <c r="L106" t="inlineStr"/>
-      <c r="M106" t="inlineStr"/>
-      <c r="N106" t="inlineStr"/>
-      <c r="O106" t="inlineStr"/>
-      <c r="P106" t="inlineStr"/>
+      <c r="L106" t="n">
+        <v>0</v>
+      </c>
+      <c r="M106" t="n">
+        <v>0</v>
+      </c>
+      <c r="N106" t="n">
+        <v>0</v>
+      </c>
+      <c r="O106" t="n">
+        <v>0</v>
+      </c>
+      <c r="P106" t="n">
+        <v>0</v>
+      </c>
       <c r="Q106" t="n">
         <v>3</v>
       </c>
@@ -6213,15 +7385,27 @@
       <c r="I107" t="n">
         <v>5</v>
       </c>
-      <c r="J107" t="inlineStr"/>
+      <c r="J107" t="n">
+        <v>0</v>
+      </c>
       <c r="K107" t="n">
         <v>13</v>
       </c>
-      <c r="L107" t="inlineStr"/>
-      <c r="M107" t="inlineStr"/>
-      <c r="N107" t="inlineStr"/>
-      <c r="O107" t="inlineStr"/>
-      <c r="P107" t="inlineStr"/>
+      <c r="L107" t="n">
+        <v>0</v>
+      </c>
+      <c r="M107" t="n">
+        <v>0</v>
+      </c>
+      <c r="N107" t="n">
+        <v>0</v>
+      </c>
+      <c r="O107" t="n">
+        <v>0</v>
+      </c>
+      <c r="P107" t="n">
+        <v>0</v>
+      </c>
       <c r="Q107" t="n">
         <v>1</v>
       </c>
@@ -6266,17 +7450,27 @@
       <c r="I108" t="n">
         <v>46</v>
       </c>
-      <c r="J108" t="inlineStr"/>
+      <c r="J108" t="n">
+        <v>0</v>
+      </c>
       <c r="K108" t="n">
         <v>59</v>
       </c>
       <c r="L108" t="n">
         <v>25</v>
       </c>
-      <c r="M108" t="inlineStr"/>
-      <c r="N108" t="inlineStr"/>
-      <c r="O108" t="inlineStr"/>
-      <c r="P108" t="inlineStr"/>
+      <c r="M108" t="n">
+        <v>0</v>
+      </c>
+      <c r="N108" t="n">
+        <v>0</v>
+      </c>
+      <c r="O108" t="n">
+        <v>0</v>
+      </c>
+      <c r="P108" t="n">
+        <v>0</v>
+      </c>
       <c r="Q108" t="n">
         <v>11</v>
       </c>
@@ -6321,17 +7515,27 @@
       <c r="I109" t="n">
         <v>18</v>
       </c>
-      <c r="J109" t="inlineStr"/>
+      <c r="J109" t="n">
+        <v>0</v>
+      </c>
       <c r="K109" t="n">
         <v>32</v>
       </c>
       <c r="L109" t="n">
         <v>3</v>
       </c>
-      <c r="M109" t="inlineStr"/>
-      <c r="N109" t="inlineStr"/>
-      <c r="O109" t="inlineStr"/>
-      <c r="P109" t="inlineStr"/>
+      <c r="M109" t="n">
+        <v>0</v>
+      </c>
+      <c r="N109" t="n">
+        <v>0</v>
+      </c>
+      <c r="O109" t="n">
+        <v>0</v>
+      </c>
+      <c r="P109" t="n">
+        <v>0</v>
+      </c>
       <c r="Q109" t="n">
         <v>1</v>
       </c>
@@ -6376,15 +7580,27 @@
       <c r="I110" t="n">
         <v>10</v>
       </c>
-      <c r="J110" t="inlineStr"/>
+      <c r="J110" t="n">
+        <v>0</v>
+      </c>
       <c r="K110" t="n">
         <v>12</v>
       </c>
-      <c r="L110" t="inlineStr"/>
-      <c r="M110" t="inlineStr"/>
-      <c r="N110" t="inlineStr"/>
-      <c r="O110" t="inlineStr"/>
-      <c r="P110" t="inlineStr"/>
+      <c r="L110" t="n">
+        <v>0</v>
+      </c>
+      <c r="M110" t="n">
+        <v>0</v>
+      </c>
+      <c r="N110" t="n">
+        <v>0</v>
+      </c>
+      <c r="O110" t="n">
+        <v>0</v>
+      </c>
+      <c r="P110" t="n">
+        <v>0</v>
+      </c>
       <c r="Q110" t="n">
         <v>0</v>
       </c>
@@ -6429,15 +7645,27 @@
       <c r="I111" t="n">
         <v>18</v>
       </c>
-      <c r="J111" t="inlineStr"/>
+      <c r="J111" t="n">
+        <v>0</v>
+      </c>
       <c r="K111" t="n">
         <v>31</v>
       </c>
-      <c r="L111" t="inlineStr"/>
-      <c r="M111" t="inlineStr"/>
-      <c r="N111" t="inlineStr"/>
-      <c r="O111" t="inlineStr"/>
-      <c r="P111" t="inlineStr"/>
+      <c r="L111" t="n">
+        <v>0</v>
+      </c>
+      <c r="M111" t="n">
+        <v>0</v>
+      </c>
+      <c r="N111" t="n">
+        <v>0</v>
+      </c>
+      <c r="O111" t="n">
+        <v>0</v>
+      </c>
+      <c r="P111" t="n">
+        <v>0</v>
+      </c>
       <c r="Q111" t="n">
         <v>3</v>
       </c>
@@ -6482,17 +7710,27 @@
       <c r="I112" t="n">
         <v>32</v>
       </c>
-      <c r="J112" t="inlineStr"/>
+      <c r="J112" t="n">
+        <v>0</v>
+      </c>
       <c r="K112" t="n">
         <v>52</v>
       </c>
       <c r="L112" t="n">
         <v>5</v>
       </c>
-      <c r="M112" t="inlineStr"/>
-      <c r="N112" t="inlineStr"/>
-      <c r="O112" t="inlineStr"/>
-      <c r="P112" t="inlineStr"/>
+      <c r="M112" t="n">
+        <v>0</v>
+      </c>
+      <c r="N112" t="n">
+        <v>0</v>
+      </c>
+      <c r="O112" t="n">
+        <v>0</v>
+      </c>
+      <c r="P112" t="n">
+        <v>0</v>
+      </c>
       <c r="Q112" t="n">
         <v>5</v>
       </c>
@@ -6537,15 +7775,27 @@
       <c r="I113" t="n">
         <v>29</v>
       </c>
-      <c r="J113" t="inlineStr"/>
+      <c r="J113" t="n">
+        <v>0</v>
+      </c>
       <c r="K113" t="n">
         <v>59</v>
       </c>
-      <c r="L113" t="inlineStr"/>
-      <c r="M113" t="inlineStr"/>
-      <c r="N113" t="inlineStr"/>
-      <c r="O113" t="inlineStr"/>
-      <c r="P113" t="inlineStr"/>
+      <c r="L113" t="n">
+        <v>0</v>
+      </c>
+      <c r="M113" t="n">
+        <v>0</v>
+      </c>
+      <c r="N113" t="n">
+        <v>0</v>
+      </c>
+      <c r="O113" t="n">
+        <v>0</v>
+      </c>
+      <c r="P113" t="n">
+        <v>0</v>
+      </c>
       <c r="Q113" t="n">
         <v>4</v>
       </c>
@@ -6590,15 +7840,27 @@
       <c r="I114" t="n">
         <v>37</v>
       </c>
-      <c r="J114" t="inlineStr"/>
-      <c r="K114" t="inlineStr"/>
+      <c r="J114" t="n">
+        <v>0</v>
+      </c>
+      <c r="K114" t="n">
+        <v>0</v>
+      </c>
       <c r="L114" t="n">
         <v>65</v>
       </c>
-      <c r="M114" t="inlineStr"/>
-      <c r="N114" t="inlineStr"/>
-      <c r="O114" t="inlineStr"/>
-      <c r="P114" t="inlineStr"/>
+      <c r="M114" t="n">
+        <v>0</v>
+      </c>
+      <c r="N114" t="n">
+        <v>0</v>
+      </c>
+      <c r="O114" t="n">
+        <v>0</v>
+      </c>
+      <c r="P114" t="n">
+        <v>0</v>
+      </c>
       <c r="Q114" t="n">
         <v>3</v>
       </c>
@@ -6643,15 +7905,27 @@
       <c r="I115" t="n">
         <v>27</v>
       </c>
-      <c r="J115" t="inlineStr"/>
-      <c r="K115" t="inlineStr"/>
+      <c r="J115" t="n">
+        <v>0</v>
+      </c>
+      <c r="K115" t="n">
+        <v>0</v>
+      </c>
       <c r="L115" t="n">
         <v>48</v>
       </c>
-      <c r="M115" t="inlineStr"/>
-      <c r="N115" t="inlineStr"/>
-      <c r="O115" t="inlineStr"/>
-      <c r="P115" t="inlineStr"/>
+      <c r="M115" t="n">
+        <v>0</v>
+      </c>
+      <c r="N115" t="n">
+        <v>0</v>
+      </c>
+      <c r="O115" t="n">
+        <v>0</v>
+      </c>
+      <c r="P115" t="n">
+        <v>0</v>
+      </c>
       <c r="Q115" t="n">
         <v>3</v>
       </c>
@@ -6705,9 +7979,15 @@
       <c r="L116" t="n">
         <v>142</v>
       </c>
-      <c r="M116" t="inlineStr"/>
-      <c r="N116" t="inlineStr"/>
-      <c r="O116" t="inlineStr"/>
+      <c r="M116" t="n">
+        <v>0</v>
+      </c>
+      <c r="N116" t="n">
+        <v>0</v>
+      </c>
+      <c r="O116" t="n">
+        <v>0</v>
+      </c>
       <c r="P116" t="n">
         <v>8</v>
       </c>
@@ -6755,16 +8035,24 @@
       <c r="I117" t="n">
         <v>60</v>
       </c>
-      <c r="J117" t="inlineStr"/>
+      <c r="J117" t="n">
+        <v>0</v>
+      </c>
       <c r="K117" t="n">
         <v>48</v>
       </c>
       <c r="L117" t="n">
         <v>59</v>
       </c>
-      <c r="M117" t="inlineStr"/>
-      <c r="N117" t="inlineStr"/>
-      <c r="O117" t="inlineStr"/>
+      <c r="M117" t="n">
+        <v>0</v>
+      </c>
+      <c r="N117" t="n">
+        <v>0</v>
+      </c>
+      <c r="O117" t="n">
+        <v>0</v>
+      </c>
       <c r="P117" t="n">
         <v>7</v>
       </c>
@@ -6812,16 +8100,30 @@
       <c r="I118" t="n">
         <v>2</v>
       </c>
-      <c r="J118" t="inlineStr"/>
+      <c r="J118" t="n">
+        <v>0</v>
+      </c>
       <c r="K118" t="n">
         <v>3</v>
       </c>
-      <c r="L118" t="inlineStr"/>
-      <c r="M118" t="inlineStr"/>
-      <c r="N118" t="inlineStr"/>
-      <c r="O118" t="inlineStr"/>
-      <c r="P118" t="inlineStr"/>
-      <c r="Q118" t="inlineStr"/>
+      <c r="L118" t="n">
+        <v>0</v>
+      </c>
+      <c r="M118" t="n">
+        <v>0</v>
+      </c>
+      <c r="N118" t="n">
+        <v>0</v>
+      </c>
+      <c r="O118" t="n">
+        <v>0</v>
+      </c>
+      <c r="P118" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q118" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -6863,15 +8165,27 @@
       <c r="I119" t="n">
         <v>12</v>
       </c>
-      <c r="J119" t="inlineStr"/>
+      <c r="J119" t="n">
+        <v>0</v>
+      </c>
       <c r="K119" t="n">
         <v>23</v>
       </c>
-      <c r="L119" t="inlineStr"/>
-      <c r="M119" t="inlineStr"/>
-      <c r="N119" t="inlineStr"/>
-      <c r="O119" t="inlineStr"/>
-      <c r="P119" t="inlineStr"/>
+      <c r="L119" t="n">
+        <v>0</v>
+      </c>
+      <c r="M119" t="n">
+        <v>0</v>
+      </c>
+      <c r="N119" t="n">
+        <v>0</v>
+      </c>
+      <c r="O119" t="n">
+        <v>0</v>
+      </c>
+      <c r="P119" t="n">
+        <v>0</v>
+      </c>
       <c r="Q119" t="n">
         <v>1</v>
       </c>
@@ -6916,15 +8230,27 @@
       <c r="I120" t="n">
         <v>22</v>
       </c>
-      <c r="J120" t="inlineStr"/>
+      <c r="J120" t="n">
+        <v>0</v>
+      </c>
       <c r="K120" t="n">
         <v>36</v>
       </c>
-      <c r="L120" t="inlineStr"/>
-      <c r="M120" t="inlineStr"/>
-      <c r="N120" t="inlineStr"/>
-      <c r="O120" t="inlineStr"/>
-      <c r="P120" t="inlineStr"/>
+      <c r="L120" t="n">
+        <v>0</v>
+      </c>
+      <c r="M120" t="n">
+        <v>0</v>
+      </c>
+      <c r="N120" t="n">
+        <v>0</v>
+      </c>
+      <c r="O120" t="n">
+        <v>0</v>
+      </c>
+      <c r="P120" t="n">
+        <v>0</v>
+      </c>
       <c r="Q120" t="n">
         <v>0</v>
       </c>
@@ -6969,15 +8295,27 @@
       <c r="I121" t="n">
         <v>17</v>
       </c>
-      <c r="J121" t="inlineStr"/>
+      <c r="J121" t="n">
+        <v>0</v>
+      </c>
       <c r="K121" t="n">
         <v>24</v>
       </c>
-      <c r="L121" t="inlineStr"/>
-      <c r="M121" t="inlineStr"/>
-      <c r="N121" t="inlineStr"/>
-      <c r="O121" t="inlineStr"/>
-      <c r="P121" t="inlineStr"/>
+      <c r="L121" t="n">
+        <v>0</v>
+      </c>
+      <c r="M121" t="n">
+        <v>0</v>
+      </c>
+      <c r="N121" t="n">
+        <v>0</v>
+      </c>
+      <c r="O121" t="n">
+        <v>0</v>
+      </c>
+      <c r="P121" t="n">
+        <v>0</v>
+      </c>
       <c r="Q121" t="n">
         <v>0</v>
       </c>
@@ -7016,16 +8354,36 @@
       <c r="G122" t="n">
         <v>0</v>
       </c>
-      <c r="H122" t="inlineStr"/>
-      <c r="I122" t="inlineStr"/>
-      <c r="J122" t="inlineStr"/>
-      <c r="K122" t="inlineStr"/>
-      <c r="L122" t="inlineStr"/>
-      <c r="M122" t="inlineStr"/>
-      <c r="N122" t="inlineStr"/>
-      <c r="O122" t="inlineStr"/>
-      <c r="P122" t="inlineStr"/>
-      <c r="Q122" t="inlineStr"/>
+      <c r="H122" t="n">
+        <v>0</v>
+      </c>
+      <c r="I122" t="n">
+        <v>0</v>
+      </c>
+      <c r="J122" t="n">
+        <v>0</v>
+      </c>
+      <c r="K122" t="n">
+        <v>0</v>
+      </c>
+      <c r="L122" t="n">
+        <v>0</v>
+      </c>
+      <c r="M122" t="n">
+        <v>0</v>
+      </c>
+      <c r="N122" t="n">
+        <v>0</v>
+      </c>
+      <c r="O122" t="n">
+        <v>0</v>
+      </c>
+      <c r="P122" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q122" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -7079,8 +8437,12 @@
       <c r="M123" t="n">
         <v>16</v>
       </c>
-      <c r="N123" t="inlineStr"/>
-      <c r="O123" t="inlineStr"/>
+      <c r="N123" t="n">
+        <v>0</v>
+      </c>
+      <c r="O123" t="n">
+        <v>0</v>
+      </c>
       <c r="P123" t="n">
         <v>9</v>
       </c>
@@ -7109,7 +8471,9 @@
           <t>Kane</t>
         </is>
       </c>
-      <c r="E124" t="inlineStr"/>
+      <c r="E124" t="n">
+        <v>0</v>
+      </c>
       <c r="F124" t="inlineStr">
         <is>
           <t>CHARTER SCH</t>
@@ -7136,8 +8500,12 @@
       <c r="M124" t="n">
         <v>13</v>
       </c>
-      <c r="N124" t="inlineStr"/>
-      <c r="O124" t="inlineStr"/>
+      <c r="N124" t="n">
+        <v>0</v>
+      </c>
+      <c r="O124" t="n">
+        <v>0</v>
+      </c>
       <c r="P124" t="n">
         <v>3</v>
       </c>
@@ -7194,9 +8562,15 @@
       <c r="L125" t="n">
         <v>61</v>
       </c>
-      <c r="M125" t="inlineStr"/>
-      <c r="N125" t="inlineStr"/>
-      <c r="O125" t="inlineStr"/>
+      <c r="M125" t="n">
+        <v>0</v>
+      </c>
+      <c r="N125" t="n">
+        <v>0</v>
+      </c>
+      <c r="O125" t="n">
+        <v>0</v>
+      </c>
       <c r="P125" t="n">
         <v>6</v>
       </c>
@@ -7244,17 +8618,27 @@
       <c r="I126" t="n">
         <v>24</v>
       </c>
-      <c r="J126" t="inlineStr"/>
+      <c r="J126" t="n">
+        <v>0</v>
+      </c>
       <c r="K126" t="n">
         <v>9</v>
       </c>
       <c r="L126" t="n">
         <v>24</v>
       </c>
-      <c r="M126" t="inlineStr"/>
-      <c r="N126" t="inlineStr"/>
-      <c r="O126" t="inlineStr"/>
-      <c r="P126" t="inlineStr"/>
+      <c r="M126" t="n">
+        <v>0</v>
+      </c>
+      <c r="N126" t="n">
+        <v>0</v>
+      </c>
+      <c r="O126" t="n">
+        <v>0</v>
+      </c>
+      <c r="P126" t="n">
+        <v>0</v>
+      </c>
       <c r="Q126" t="n">
         <v>0</v>
       </c>
@@ -7302,15 +8686,21 @@
       <c r="J127" t="n">
         <v>103</v>
       </c>
-      <c r="K127" t="inlineStr"/>
+      <c r="K127" t="n">
+        <v>0</v>
+      </c>
       <c r="L127" t="n">
         <v>6</v>
       </c>
       <c r="M127" t="n">
         <v>22</v>
       </c>
-      <c r="N127" t="inlineStr"/>
-      <c r="O127" t="inlineStr"/>
+      <c r="N127" t="n">
+        <v>0</v>
+      </c>
+      <c r="O127" t="n">
+        <v>0</v>
+      </c>
       <c r="P127" t="n">
         <v>12</v>
       </c>
@@ -7358,17 +8748,27 @@
       <c r="I128" t="n">
         <v>68</v>
       </c>
-      <c r="J128" t="inlineStr"/>
+      <c r="J128" t="n">
+        <v>0</v>
+      </c>
       <c r="K128" t="n">
         <v>11</v>
       </c>
       <c r="L128" t="n">
         <v>99</v>
       </c>
-      <c r="M128" t="inlineStr"/>
-      <c r="N128" t="inlineStr"/>
-      <c r="O128" t="inlineStr"/>
-      <c r="P128" t="inlineStr"/>
+      <c r="M128" t="n">
+        <v>0</v>
+      </c>
+      <c r="N128" t="n">
+        <v>0</v>
+      </c>
+      <c r="O128" t="n">
+        <v>0</v>
+      </c>
+      <c r="P128" t="n">
+        <v>0</v>
+      </c>
       <c r="Q128" t="n">
         <v>12</v>
       </c>
@@ -7413,14 +8813,24 @@
       <c r="I129" t="n">
         <v>16</v>
       </c>
-      <c r="J129" t="inlineStr"/>
+      <c r="J129" t="n">
+        <v>0</v>
+      </c>
       <c r="K129" t="n">
         <v>26</v>
       </c>
-      <c r="L129" t="inlineStr"/>
-      <c r="M129" t="inlineStr"/>
-      <c r="N129" t="inlineStr"/>
-      <c r="O129" t="inlineStr"/>
+      <c r="L129" t="n">
+        <v>0</v>
+      </c>
+      <c r="M129" t="n">
+        <v>0</v>
+      </c>
+      <c r="N129" t="n">
+        <v>0</v>
+      </c>
+      <c r="O129" t="n">
+        <v>0</v>
+      </c>
       <c r="P129" t="n">
         <v>2</v>
       </c>
@@ -7477,9 +8887,15 @@
       <c r="L130" t="n">
         <v>5</v>
       </c>
-      <c r="M130" t="inlineStr"/>
-      <c r="N130" t="inlineStr"/>
-      <c r="O130" t="inlineStr"/>
+      <c r="M130" t="n">
+        <v>0</v>
+      </c>
+      <c r="N130" t="n">
+        <v>0</v>
+      </c>
+      <c r="O130" t="n">
+        <v>0</v>
+      </c>
       <c r="P130" t="n">
         <v>2</v>
       </c>
@@ -7527,16 +8943,30 @@
       <c r="I131" t="n">
         <v>0</v>
       </c>
-      <c r="J131" t="inlineStr"/>
+      <c r="J131" t="n">
+        <v>0</v>
+      </c>
       <c r="K131" t="n">
         <v>1</v>
       </c>
-      <c r="L131" t="inlineStr"/>
-      <c r="M131" t="inlineStr"/>
-      <c r="N131" t="inlineStr"/>
-      <c r="O131" t="inlineStr"/>
-      <c r="P131" t="inlineStr"/>
-      <c r="Q131" t="inlineStr"/>
+      <c r="L131" t="n">
+        <v>0</v>
+      </c>
+      <c r="M131" t="n">
+        <v>0</v>
+      </c>
+      <c r="N131" t="n">
+        <v>0</v>
+      </c>
+      <c r="O131" t="n">
+        <v>0</v>
+      </c>
+      <c r="P131" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q131" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -7584,10 +9014,18 @@
       <c r="K132" t="n">
         <v>11</v>
       </c>
-      <c r="L132" t="inlineStr"/>
-      <c r="M132" t="inlineStr"/>
-      <c r="N132" t="inlineStr"/>
-      <c r="O132" t="inlineStr"/>
+      <c r="L132" t="n">
+        <v>0</v>
+      </c>
+      <c r="M132" t="n">
+        <v>0</v>
+      </c>
+      <c r="N132" t="n">
+        <v>0</v>
+      </c>
+      <c r="O132" t="n">
+        <v>0</v>
+      </c>
       <c r="P132" t="n">
         <v>12</v>
       </c>

</xml_diff>